<commit_message>
TS 1.4 Padam input Raja final 2082 11/10/2021
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Padam Input Templates/TS 1.4 Padam Input Template.xlsx
+++ b/TS Jatai Working/Padam Input Templates/TS 1.4 Padam Input Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\texts\TS Jatai Working\Padam Input Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23B9D2AC-916E-4824-8DCA-8025305D9D79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2019ED23-ECA7-4AD2-B406-D5A3F36611A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6741" uniqueCount="1499">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6745" uniqueCount="1498">
   <si>
     <t>Passage</t>
   </si>
@@ -4010,9 +4010,6 @@
   </si>
   <si>
     <t>BrAja#svataq itiq BrAja#svate</t>
-  </si>
-  <si>
-    <t>pyAqyaqsveti# pyAyqsva</t>
   </si>
   <si>
     <t>UqtiBiqrityUqti - BiqH</t>
@@ -4680,7 +4677,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -4696,6 +4693,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4727,7 +4730,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -4928,6 +4931,12 @@
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5211,10 +5220,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V1812"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="V117" sqref="V117"/>
+      <selection pane="bottomLeft" activeCell="O1402" sqref="O1402"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -32642,7 +32651,9 @@
       <c r="N674" s="39" t="s">
         <v>521</v>
       </c>
-      <c r="O674" s="6"/>
+      <c r="O674" s="71" t="s">
+        <v>72</v>
+      </c>
       <c r="P674" s="7"/>
       <c r="Q674" s="7"/>
       <c r="R674" s="7"/>
@@ -39682,7 +39693,9 @@
       <c r="N859" s="39" t="s">
         <v>624</v>
       </c>
-      <c r="O859" s="6"/>
+      <c r="O859" s="71" t="s">
+        <v>74</v>
+      </c>
       <c r="P859" s="7"/>
       <c r="Q859" s="7"/>
       <c r="R859" s="7"/>
@@ -43611,9 +43624,7 @@
       <c r="S963" s="7"/>
       <c r="T963" s="7"/>
       <c r="U963" s="7"/>
-      <c r="V963" s="39" t="s">
-        <v>1325</v>
-      </c>
+      <c r="V963" s="70"/>
     </row>
     <row r="964" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="E964" s="18"/>
@@ -43764,7 +43775,7 @@
       <c r="T967" s="7"/>
       <c r="U967" s="7"/>
       <c r="V967" s="39" t="s">
-        <v>1326</v>
+        <v>1325</v>
       </c>
     </row>
     <row r="968" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -43881,7 +43892,7 @@
       <c r="T970" s="7"/>
       <c r="U970" s="7"/>
       <c r="V970" s="40" t="s">
-        <v>1327</v>
+        <v>1326</v>
       </c>
     </row>
     <row r="971" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -44047,7 +44058,7 @@
       <c r="T974" s="7"/>
       <c r="U974" s="7"/>
       <c r="V974" s="39" t="s">
-        <v>1328</v>
+        <v>1327</v>
       </c>
     </row>
     <row r="975" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -44123,7 +44134,7 @@
       <c r="T976" s="7"/>
       <c r="U976" s="7"/>
       <c r="V976" s="39" t="s">
-        <v>1329</v>
+        <v>1328</v>
       </c>
     </row>
     <row r="977" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -44199,7 +44210,7 @@
       <c r="T978" s="7"/>
       <c r="U978" s="7"/>
       <c r="V978" s="39" t="s">
-        <v>1330</v>
+        <v>1329</v>
       </c>
     </row>
     <row r="979" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -44379,7 +44390,7 @@
       <c r="T982" s="7"/>
       <c r="U982" s="7"/>
       <c r="V982" s="39" t="s">
-        <v>1331</v>
+        <v>1330</v>
       </c>
     </row>
     <row r="983" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -44463,7 +44474,7 @@
       <c r="T984" s="7"/>
       <c r="U984" s="7"/>
       <c r="V984" s="40" t="s">
-        <v>1332</v>
+        <v>1331</v>
       </c>
     </row>
     <row r="985" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -44660,7 +44671,7 @@
       <c r="T989" s="7"/>
       <c r="U989" s="7"/>
       <c r="V989" s="39" t="s">
-        <v>1333</v>
+        <v>1332</v>
       </c>
     </row>
     <row r="990" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -44808,7 +44819,7 @@
       <c r="T993" s="7"/>
       <c r="U993" s="7"/>
       <c r="V993" s="39" t="s">
-        <v>1334</v>
+        <v>1333</v>
       </c>
     </row>
     <row r="994" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -44921,7 +44932,7 @@
       <c r="T996" s="7"/>
       <c r="U996" s="7"/>
       <c r="V996" s="39" t="s">
-        <v>1335</v>
+        <v>1334</v>
       </c>
     </row>
     <row r="997" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -45258,7 +45269,7 @@
       <c r="T1005" s="7"/>
       <c r="U1005" s="7"/>
       <c r="V1005" s="39" t="s">
-        <v>1336</v>
+        <v>1335</v>
       </c>
     </row>
     <row r="1006" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -45706,7 +45717,7 @@
       <c r="T1017" s="7"/>
       <c r="U1017" s="7"/>
       <c r="V1017" s="39" t="s">
-        <v>1337</v>
+        <v>1336</v>
       </c>
     </row>
     <row r="1018" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -46006,7 +46017,7 @@
       <c r="T1025" s="7"/>
       <c r="U1025" s="7"/>
       <c r="V1025" s="39" t="s">
-        <v>1338</v>
+        <v>1337</v>
       </c>
     </row>
     <row r="1026" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -46043,7 +46054,7 @@
       <c r="T1026" s="7"/>
       <c r="U1026" s="7"/>
       <c r="V1026" s="39" t="s">
-        <v>1339</v>
+        <v>1338</v>
       </c>
     </row>
     <row r="1027" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -46119,7 +46130,7 @@
       <c r="T1028" s="7"/>
       <c r="U1028" s="7"/>
       <c r="V1028" s="39" t="s">
-        <v>1340</v>
+        <v>1339</v>
       </c>
     </row>
     <row r="1029" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -46195,7 +46206,7 @@
       <c r="T1030" s="7"/>
       <c r="U1030" s="7"/>
       <c r="V1030" s="39" t="s">
-        <v>1341</v>
+        <v>1340</v>
       </c>
     </row>
     <row r="1031" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -46271,7 +46282,7 @@
       <c r="T1032" s="7"/>
       <c r="U1032" s="7"/>
       <c r="V1032" s="39" t="s">
-        <v>1342</v>
+        <v>1341</v>
       </c>
     </row>
     <row r="1033" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -46347,7 +46358,7 @@
       <c r="T1034" s="7"/>
       <c r="U1034" s="7"/>
       <c r="V1034" s="39" t="s">
-        <v>1343</v>
+        <v>1342</v>
       </c>
     </row>
     <row r="1035" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -46423,7 +46434,7 @@
       <c r="T1036" s="7"/>
       <c r="U1036" s="7"/>
       <c r="V1036" s="39" t="s">
-        <v>1344</v>
+        <v>1343</v>
       </c>
     </row>
     <row r="1037" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -46795,7 +46806,7 @@
       <c r="T1046" s="7"/>
       <c r="U1046" s="7"/>
       <c r="V1046" s="40" t="s">
-        <v>1345</v>
+        <v>1344</v>
       </c>
     </row>
     <row r="1047" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -46982,7 +46993,7 @@
       <c r="T1051" s="7"/>
       <c r="U1051" s="7"/>
       <c r="V1051" s="39" t="s">
-        <v>1346</v>
+        <v>1345</v>
       </c>
     </row>
     <row r="1052" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -47169,7 +47180,7 @@
       <c r="T1056" s="7"/>
       <c r="U1056" s="7"/>
       <c r="V1056" s="39" t="s">
-        <v>1347</v>
+        <v>1346</v>
       </c>
     </row>
     <row r="1057" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -47208,7 +47219,7 @@
       <c r="T1057" s="7"/>
       <c r="U1057" s="7"/>
       <c r="V1057" s="39" t="s">
-        <v>1348</v>
+        <v>1347</v>
       </c>
     </row>
     <row r="1058" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -47469,7 +47480,7 @@
       <c r="T1064" s="7"/>
       <c r="U1064" s="7"/>
       <c r="V1064" s="39" t="s">
-        <v>1349</v>
+        <v>1348</v>
       </c>
     </row>
     <row r="1065" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -47508,7 +47519,7 @@
       <c r="T1065" s="7"/>
       <c r="U1065" s="7"/>
       <c r="V1065" s="39" t="s">
-        <v>1350</v>
+        <v>1349</v>
       </c>
     </row>
     <row r="1066" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -47547,7 +47558,7 @@
       <c r="T1066" s="7"/>
       <c r="U1066" s="7"/>
       <c r="V1066" s="39" t="s">
-        <v>1351</v>
+        <v>1350</v>
       </c>
     </row>
     <row r="1067" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -47588,7 +47599,7 @@
       <c r="T1067" s="7"/>
       <c r="U1067" s="7"/>
       <c r="V1067" s="39" t="s">
-        <v>1352</v>
+        <v>1351</v>
       </c>
     </row>
     <row r="1068" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -47707,7 +47718,7 @@
       <c r="T1070" s="7"/>
       <c r="U1070" s="7"/>
       <c r="V1070" s="39" t="s">
-        <v>1353</v>
+        <v>1352</v>
       </c>
     </row>
     <row r="1071" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -48162,7 +48173,7 @@
       <c r="T1082" s="7"/>
       <c r="U1082" s="7"/>
       <c r="V1082" s="39" t="s">
-        <v>1354</v>
+        <v>1353</v>
       </c>
     </row>
     <row r="1083" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -48573,7 +48584,7 @@
       <c r="T1093" s="7"/>
       <c r="U1093" s="7"/>
       <c r="V1093" s="51" t="s">
-        <v>1355</v>
+        <v>1354</v>
       </c>
     </row>
     <row r="1094" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -48680,7 +48691,9 @@
       <c r="N1096" s="39" t="s">
         <v>747</v>
       </c>
-      <c r="O1096" s="6"/>
+      <c r="O1096" s="71" t="s">
+        <v>74</v>
+      </c>
       <c r="P1096" s="7"/>
       <c r="Q1096" s="7"/>
       <c r="R1096" s="7"/>
@@ -48768,7 +48781,7 @@
       <c r="T1098" s="7"/>
       <c r="U1098" s="7"/>
       <c r="V1098" s="39" t="s">
-        <v>1356</v>
+        <v>1355</v>
       </c>
     </row>
     <row r="1099" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -49031,7 +49044,7 @@
       <c r="T1105" s="7"/>
       <c r="U1105" s="7"/>
       <c r="V1105" s="39" t="s">
-        <v>1357</v>
+        <v>1356</v>
       </c>
     </row>
     <row r="1106" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -49442,7 +49455,7 @@
       <c r="T1116" s="7"/>
       <c r="U1116" s="7"/>
       <c r="V1116" s="39" t="s">
-        <v>1355</v>
+        <v>1354</v>
       </c>
     </row>
     <row r="1117" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -49748,7 +49761,7 @@
       <c r="T1124" s="7"/>
       <c r="U1124" s="7"/>
       <c r="V1124" s="39" t="s">
-        <v>1358</v>
+        <v>1357</v>
       </c>
     </row>
     <row r="1125" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -50056,7 +50069,7 @@
       <c r="T1132" s="7"/>
       <c r="U1132" s="7"/>
       <c r="V1132" s="39" t="s">
-        <v>1359</v>
+        <v>1358</v>
       </c>
     </row>
     <row r="1133" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -50467,7 +50480,7 @@
       <c r="T1143" s="7"/>
       <c r="U1143" s="7"/>
       <c r="V1143" s="39" t="s">
-        <v>1355</v>
+        <v>1354</v>
       </c>
     </row>
     <row r="1144" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -50541,7 +50554,7 @@
       <c r="T1145" s="7"/>
       <c r="U1145" s="7"/>
       <c r="V1145" s="39" t="s">
-        <v>1360</v>
+        <v>1359</v>
       </c>
     </row>
     <row r="1146" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -50654,7 +50667,7 @@
       <c r="T1148" s="7"/>
       <c r="U1148" s="7"/>
       <c r="V1148" s="39" t="s">
-        <v>1361</v>
+        <v>1360</v>
       </c>
     </row>
     <row r="1149" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -50732,7 +50745,7 @@
       <c r="T1150" s="7"/>
       <c r="U1150" s="7"/>
       <c r="V1150" s="39" t="s">
-        <v>1362</v>
+        <v>1361</v>
       </c>
     </row>
     <row r="1151" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -50845,7 +50858,7 @@
       <c r="S1153" s="7"/>
       <c r="T1153" s="7"/>
       <c r="V1153" s="39" t="s">
-        <v>1363</v>
+        <v>1362</v>
       </c>
     </row>
     <row r="1154" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -51036,7 +51049,7 @@
       <c r="T1158" s="7"/>
       <c r="U1158" s="7"/>
       <c r="V1158" s="39" t="s">
-        <v>1364</v>
+        <v>1363</v>
       </c>
     </row>
     <row r="1159" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -51447,7 +51460,7 @@
       <c r="T1169" s="7"/>
       <c r="U1169" s="7"/>
       <c r="V1169" s="39" t="s">
-        <v>1355</v>
+        <v>1354</v>
       </c>
     </row>
     <row r="1170" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -51562,7 +51575,7 @@
       <c r="T1172" s="7"/>
       <c r="U1172" s="7"/>
       <c r="V1172" s="39" t="s">
-        <v>1365</v>
+        <v>1364</v>
       </c>
     </row>
     <row r="1173" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -51675,7 +51688,7 @@
       <c r="T1175" s="7"/>
       <c r="U1175" s="7"/>
       <c r="V1175" s="39" t="s">
-        <v>1366</v>
+        <v>1365</v>
       </c>
     </row>
     <row r="1176" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -51788,7 +51801,7 @@
       <c r="T1178" s="7"/>
       <c r="U1178" s="7"/>
       <c r="V1178" s="39" t="s">
-        <v>1367</v>
+        <v>1366</v>
       </c>
     </row>
     <row r="1179" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -52012,7 +52025,7 @@
       <c r="T1184" s="7"/>
       <c r="U1184" s="7"/>
       <c r="V1184" s="39" t="s">
-        <v>1368</v>
+        <v>1367</v>
       </c>
     </row>
     <row r="1185" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -52423,7 +52436,7 @@
       <c r="T1195" s="7"/>
       <c r="U1195" s="7"/>
       <c r="V1195" s="39" t="s">
-        <v>1355</v>
+        <v>1354</v>
       </c>
     </row>
     <row r="1196" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -52526,7 +52539,9 @@
       <c r="N1198" s="39" t="s">
         <v>783</v>
       </c>
-      <c r="O1198" s="6"/>
+      <c r="O1198" s="71" t="s">
+        <v>72</v>
+      </c>
       <c r="P1198" s="7"/>
       <c r="Q1198" s="7"/>
       <c r="R1198" s="7"/>
@@ -52534,7 +52549,7 @@
       <c r="T1198" s="7"/>
       <c r="U1198" s="7"/>
       <c r="V1198" s="39" t="s">
-        <v>1369</v>
+        <v>1368</v>
       </c>
     </row>
     <row r="1199" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -52573,7 +52588,7 @@
       <c r="T1199" s="7"/>
       <c r="U1199" s="7"/>
       <c r="V1199" s="39" t="s">
-        <v>1370</v>
+        <v>1369</v>
       </c>
     </row>
     <row r="1200" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -52686,7 +52701,7 @@
       <c r="T1202" s="7"/>
       <c r="U1202" s="7"/>
       <c r="V1202" s="39" t="s">
-        <v>1353</v>
+        <v>1352</v>
       </c>
     </row>
     <row r="1203" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -52762,7 +52777,7 @@
       <c r="T1204" s="7"/>
       <c r="U1204" s="7"/>
       <c r="V1204" s="39" t="s">
-        <v>1371</v>
+        <v>1370</v>
       </c>
     </row>
     <row r="1205" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -53150,7 +53165,7 @@
       <c r="T1214" s="7"/>
       <c r="U1214" s="7"/>
       <c r="V1214" s="39" t="s">
-        <v>1372</v>
+        <v>1371</v>
       </c>
     </row>
     <row r="1215" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -53561,7 +53576,7 @@
       <c r="T1225" s="7"/>
       <c r="U1225" s="7"/>
       <c r="V1225" s="51" t="s">
-        <v>1355</v>
+        <v>1354</v>
       </c>
     </row>
     <row r="1226" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -53699,8 +53714,7 @@
       <c r="N1229" s="39" t="s">
         <v>797</v>
       </c>
-      <c r="O1229" s="6"/>
-      <c r="P1229" s="6" t="s">
+      <c r="O1229" s="6" t="s">
         <v>72</v>
       </c>
       <c r="Q1229" s="7"/>
@@ -53709,7 +53723,7 @@
       <c r="T1229" s="7"/>
       <c r="U1229" s="7"/>
       <c r="V1229" s="39" t="s">
-        <v>1373</v>
+        <v>1372</v>
       </c>
     </row>
     <row r="1230" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -53935,7 +53949,7 @@
       <c r="T1235" s="7"/>
       <c r="U1235" s="7"/>
       <c r="V1235" s="39" t="s">
-        <v>1374</v>
+        <v>1373</v>
       </c>
     </row>
     <row r="1236" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -54270,7 +54284,7 @@
       <c r="T1244" s="7"/>
       <c r="U1244" s="7"/>
       <c r="V1244" s="39" t="s">
-        <v>1375</v>
+        <v>1374</v>
       </c>
     </row>
     <row r="1245" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -54617,7 +54631,7 @@
       <c r="T1253" s="7"/>
       <c r="U1253" s="7"/>
       <c r="V1253" s="39" t="s">
-        <v>1376</v>
+        <v>1375</v>
       </c>
     </row>
     <row r="1254" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -54734,7 +54748,7 @@
       <c r="T1256" s="7"/>
       <c r="U1256" s="7"/>
       <c r="V1256" s="39" t="s">
-        <v>1377</v>
+        <v>1376</v>
       </c>
     </row>
     <row r="1257" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -54962,7 +54976,7 @@
       <c r="T1262" s="7"/>
       <c r="U1262" s="7"/>
       <c r="V1262" s="39" t="s">
-        <v>1371</v>
+        <v>1370</v>
       </c>
     </row>
     <row r="1263" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -55223,7 +55237,7 @@
       <c r="T1269" s="7"/>
       <c r="U1269" s="7"/>
       <c r="V1269" s="39" t="s">
-        <v>1378</v>
+        <v>1377</v>
       </c>
     </row>
     <row r="1270" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -55262,7 +55276,7 @@
       <c r="T1270" s="7"/>
       <c r="U1270" s="7"/>
       <c r="V1270" s="39" t="s">
-        <v>1379</v>
+        <v>1378</v>
       </c>
     </row>
     <row r="1271" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -55729,7 +55743,7 @@
       <c r="T1282" s="7"/>
       <c r="U1282" s="7"/>
       <c r="V1282" s="39" t="s">
-        <v>1380</v>
+        <v>1379</v>
       </c>
     </row>
     <row r="1283" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -55842,7 +55856,7 @@
       <c r="T1285" s="7"/>
       <c r="U1285" s="7"/>
       <c r="V1285" s="39" t="s">
-        <v>1381</v>
+        <v>1380</v>
       </c>
     </row>
     <row r="1286" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -56048,7 +56062,7 @@
       <c r="T1290" s="7"/>
       <c r="U1290" s="7"/>
       <c r="V1290" s="39" t="s">
-        <v>1382</v>
+        <v>1381</v>
       </c>
     </row>
     <row r="1291" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -56323,7 +56337,7 @@
       <c r="T1297" s="7"/>
       <c r="U1297" s="7"/>
       <c r="V1297" s="39" t="s">
-        <v>1383</v>
+        <v>1382</v>
       </c>
     </row>
     <row r="1298" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -56660,7 +56674,7 @@
       <c r="T1306" s="7"/>
       <c r="U1306" s="7"/>
       <c r="V1306" s="39" t="s">
-        <v>1384</v>
+        <v>1383</v>
       </c>
     </row>
     <row r="1307" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -57032,7 +57046,7 @@
       <c r="T1316" s="7"/>
       <c r="U1316" s="7"/>
       <c r="V1316" s="39" t="s">
-        <v>1385</v>
+        <v>1384</v>
       </c>
     </row>
     <row r="1317" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -57071,7 +57085,7 @@
       <c r="T1317" s="7"/>
       <c r="U1317" s="7"/>
       <c r="V1317" s="39" t="s">
-        <v>1386</v>
+        <v>1385</v>
       </c>
     </row>
     <row r="1318" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -57110,7 +57124,7 @@
       <c r="T1318" s="7"/>
       <c r="U1318" s="7"/>
       <c r="V1318" s="39" t="s">
-        <v>1387</v>
+        <v>1386</v>
       </c>
     </row>
     <row r="1319" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -57416,7 +57430,7 @@
       <c r="T1326" s="7"/>
       <c r="U1326" s="7"/>
       <c r="V1326" s="39" t="s">
-        <v>1388</v>
+        <v>1387</v>
       </c>
     </row>
     <row r="1327" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -57570,7 +57584,7 @@
       <c r="T1330" s="7"/>
       <c r="U1330" s="7"/>
       <c r="V1330" s="39" t="s">
-        <v>1389</v>
+        <v>1388</v>
       </c>
     </row>
     <row r="1331" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -57685,7 +57699,7 @@
       <c r="S1333" s="7"/>
       <c r="T1333" s="7"/>
       <c r="V1333" s="39" t="s">
-        <v>1390</v>
+        <v>1389</v>
       </c>
     </row>
     <row r="1334" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -57760,7 +57774,7 @@
       <c r="S1335" s="7"/>
       <c r="T1335" s="7"/>
       <c r="V1335" s="40" t="s">
-        <v>1391</v>
+        <v>1390</v>
       </c>
     </row>
     <row r="1336" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -57873,7 +57887,7 @@
       <c r="T1338" s="7"/>
       <c r="U1338" s="7"/>
       <c r="V1338" s="39" t="s">
-        <v>1392</v>
+        <v>1391</v>
       </c>
     </row>
     <row r="1339" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -58062,7 +58076,7 @@
       <c r="T1343" s="7"/>
       <c r="U1343" s="7"/>
       <c r="V1343" s="53" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
     </row>
     <row r="1344" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -58306,7 +58320,7 @@
       <c r="T1349" s="7"/>
       <c r="U1349" s="7"/>
       <c r="V1349" s="39" t="s">
-        <v>1394</v>
+        <v>1393</v>
       </c>
     </row>
     <row r="1350" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -58348,7 +58362,7 @@
       <c r="T1350" s="7"/>
       <c r="U1350" s="7"/>
       <c r="V1350" s="39" t="s">
-        <v>1395</v>
+        <v>1394</v>
       </c>
     </row>
     <row r="1351" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -58432,7 +58446,7 @@
         <v>82</v>
       </c>
       <c r="V1352" s="39" t="s">
-        <v>1396</v>
+        <v>1395</v>
       </c>
     </row>
     <row r="1353" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -58554,7 +58568,7 @@
       <c r="T1355" s="7"/>
       <c r="U1355" s="7"/>
       <c r="V1355" s="39" t="s">
-        <v>1397</v>
+        <v>1396</v>
       </c>
     </row>
     <row r="1356" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -58596,7 +58610,7 @@
       <c r="T1356" s="7"/>
       <c r="U1356" s="7"/>
       <c r="V1356" s="39" t="s">
-        <v>1398</v>
+        <v>1397</v>
       </c>
     </row>
     <row r="1357" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -58718,7 +58732,7 @@
       <c r="T1359" s="7"/>
       <c r="U1359" s="7"/>
       <c r="V1359" s="39" t="s">
-        <v>1399</v>
+        <v>1398</v>
       </c>
     </row>
     <row r="1360" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -59048,7 +59062,7 @@
       <c r="T1367" s="7"/>
       <c r="U1367" s="7"/>
       <c r="V1367" s="39" t="s">
-        <v>1400</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="1368" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -59174,7 +59188,7 @@
       <c r="T1370" s="7"/>
       <c r="U1370" s="7"/>
       <c r="V1370" s="39" t="s">
-        <v>1401</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="1371" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -59298,7 +59312,7 @@
       <c r="T1373" s="7"/>
       <c r="U1373" s="7"/>
       <c r="V1373" s="39" t="s">
-        <v>1402</v>
+        <v>1401</v>
       </c>
     </row>
     <row r="1374" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -59502,7 +59516,7 @@
       <c r="T1378" s="7"/>
       <c r="U1378" s="7"/>
       <c r="V1378" s="39" t="s">
-        <v>1403</v>
+        <v>1402</v>
       </c>
     </row>
     <row r="1379" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -59544,7 +59558,7 @@
       <c r="T1379" s="7"/>
       <c r="U1379" s="7"/>
       <c r="V1379" s="39" t="s">
-        <v>1404</v>
+        <v>1403</v>
       </c>
     </row>
     <row r="1380" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -59912,7 +59926,7 @@
       <c r="T1388" s="7"/>
       <c r="U1388" s="7"/>
       <c r="V1388" s="39" t="s">
-        <v>1405</v>
+        <v>1404</v>
       </c>
     </row>
     <row r="1389" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -60319,7 +60333,7 @@
       <c r="T1398" s="7"/>
       <c r="U1398" s="7"/>
       <c r="V1398" s="39" t="s">
-        <v>1406</v>
+        <v>1405</v>
       </c>
     </row>
     <row r="1399" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -60473,7 +60487,9 @@
       <c r="N1402" s="51" t="s">
         <v>903</v>
       </c>
-      <c r="O1402" s="6"/>
+      <c r="O1402" s="71" t="s">
+        <v>72</v>
+      </c>
       <c r="P1402" s="7"/>
       <c r="Q1402" s="7"/>
       <c r="R1402" s="7"/>
@@ -60737,7 +60753,7 @@
       <c r="T1408" s="7"/>
       <c r="U1408" s="7"/>
       <c r="V1408" s="39" t="s">
-        <v>1407</v>
+        <v>1406</v>
       </c>
     </row>
     <row r="1409" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -60989,7 +61005,7 @@
       <c r="T1414" s="7"/>
       <c r="U1414" s="7"/>
       <c r="V1414" s="39" t="s">
-        <v>1408</v>
+        <v>1407</v>
       </c>
     </row>
     <row r="1415" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -61153,7 +61169,7 @@
       <c r="T1418" s="7"/>
       <c r="U1418" s="7"/>
       <c r="V1418" s="39" t="s">
-        <v>1371</v>
+        <v>1370</v>
       </c>
     </row>
     <row r="1419" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -61195,7 +61211,7 @@
       <c r="T1419" s="7"/>
       <c r="U1419" s="7"/>
       <c r="V1419" s="39" t="s">
-        <v>1409</v>
+        <v>1408</v>
       </c>
     </row>
     <row r="1420" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -61439,7 +61455,7 @@
       <c r="T1425" s="7"/>
       <c r="U1425" s="7"/>
       <c r="V1425" s="39" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
     </row>
     <row r="1426" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -61561,7 +61577,7 @@
       <c r="T1428" s="7"/>
       <c r="U1428" s="7"/>
       <c r="V1428" s="39" t="s">
-        <v>1411</v>
+        <v>1410</v>
       </c>
     </row>
     <row r="1429" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -61771,7 +61787,7 @@
         <v>86</v>
       </c>
       <c r="V1433" s="39" t="s">
-        <v>1412</v>
+        <v>1411</v>
       </c>
     </row>
     <row r="1434" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -61899,7 +61915,7 @@
       <c r="T1436" s="7"/>
       <c r="U1436" s="7"/>
       <c r="V1436" s="39" t="s">
-        <v>1413</v>
+        <v>1412</v>
       </c>
     </row>
     <row r="1437" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -62416,7 +62432,7 @@
       <c r="T1448" s="7"/>
       <c r="U1448" s="7"/>
       <c r="V1448" s="51" t="s">
-        <v>1414</v>
+        <v>1413</v>
       </c>
     </row>
     <row r="1449" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -62782,7 +62798,7 @@
       <c r="T1457" s="7"/>
       <c r="U1457" s="7"/>
       <c r="V1457" s="39" t="s">
-        <v>1415</v>
+        <v>1414</v>
       </c>
     </row>
     <row r="1458" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -63306,7 +63322,7 @@
       <c r="T1470" s="7"/>
       <c r="U1470" s="7"/>
       <c r="V1470" s="39" t="s">
-        <v>1416</v>
+        <v>1415</v>
       </c>
     </row>
     <row r="1471" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -63348,7 +63364,7 @@
       <c r="T1471" s="7"/>
       <c r="U1471" s="7"/>
       <c r="V1471" s="39" t="s">
-        <v>1417</v>
+        <v>1416</v>
       </c>
     </row>
     <row r="1472" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -63390,7 +63406,7 @@
       <c r="T1472" s="7"/>
       <c r="U1472" s="7"/>
       <c r="V1472" s="39" t="s">
-        <v>1418</v>
+        <v>1417</v>
       </c>
     </row>
     <row r="1473" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -63512,7 +63528,7 @@
       <c r="T1475" s="7"/>
       <c r="U1475" s="7"/>
       <c r="V1475" s="39" t="s">
-        <v>1419</v>
+        <v>1418</v>
       </c>
     </row>
     <row r="1476" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -64158,7 +64174,7 @@
       <c r="T1491" s="7"/>
       <c r="U1491" s="7"/>
       <c r="V1491" s="51" t="s">
-        <v>1420</v>
+        <v>1419</v>
       </c>
     </row>
     <row r="1492" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -64458,7 +64474,7 @@
       <c r="T1499" s="7"/>
       <c r="U1499" s="7"/>
       <c r="V1499" s="39" t="s">
-        <v>1421</v>
+        <v>1420</v>
       </c>
     </row>
     <row r="1500" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -64499,7 +64515,7 @@
       <c r="T1500" s="7"/>
       <c r="U1500" s="7"/>
       <c r="V1500" s="51" t="s">
-        <v>1422</v>
+        <v>1421</v>
       </c>
     </row>
     <row r="1501" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -64618,7 +64634,7 @@
       <c r="T1503" s="7"/>
       <c r="U1503" s="7"/>
       <c r="V1503" s="39" t="s">
-        <v>1423</v>
+        <v>1422</v>
       </c>
     </row>
     <row r="1504" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -64741,7 +64757,7 @@
       <c r="T1506" s="7"/>
       <c r="U1506" s="7"/>
       <c r="V1506" s="39" t="s">
-        <v>1424</v>
+        <v>1423</v>
       </c>
     </row>
     <row r="1507" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -64782,7 +64798,7 @@
       <c r="T1507" s="7"/>
       <c r="U1507" s="7"/>
       <c r="V1507" s="40" t="s">
-        <v>1425</v>
+        <v>1424</v>
       </c>
     </row>
     <row r="1508" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -64823,7 +64839,7 @@
       <c r="T1508" s="7"/>
       <c r="U1508" s="7"/>
       <c r="V1508" s="39" t="s">
-        <v>1426</v>
+        <v>1425</v>
       </c>
     </row>
     <row r="1509" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -65204,7 +65220,7 @@
         <v>82</v>
       </c>
       <c r="V1518" s="39" t="s">
-        <v>1427</v>
+        <v>1426</v>
       </c>
     </row>
     <row r="1519" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -65317,7 +65333,7 @@
       <c r="T1521" s="7"/>
       <c r="U1521" s="7"/>
       <c r="V1521" s="39" t="s">
-        <v>1428</v>
+        <v>1427</v>
       </c>
     </row>
     <row r="1522" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -65580,7 +65596,7 @@
       <c r="T1528" s="7"/>
       <c r="U1528" s="7"/>
       <c r="V1528" s="39" t="s">
-        <v>1429</v>
+        <v>1428</v>
       </c>
     </row>
     <row r="1529" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -65619,7 +65635,7 @@
       <c r="T1529" s="7"/>
       <c r="U1529" s="7"/>
       <c r="V1529" s="39" t="s">
-        <v>1430</v>
+        <v>1429</v>
       </c>
     </row>
     <row r="1530" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -65882,7 +65898,7 @@
       <c r="T1536" s="7"/>
       <c r="U1536" s="7"/>
       <c r="V1536" s="39" t="s">
-        <v>1431</v>
+        <v>1430</v>
       </c>
     </row>
     <row r="1537" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -66001,7 +66017,7 @@
       <c r="T1539" s="7"/>
       <c r="U1539" s="7"/>
       <c r="V1539" s="39" t="s">
-        <v>1432</v>
+        <v>1431</v>
       </c>
     </row>
     <row r="1540" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -66079,7 +66095,7 @@
       <c r="T1541" s="7"/>
       <c r="U1541" s="7"/>
       <c r="V1541" s="39" t="s">
-        <v>1433</v>
+        <v>1432</v>
       </c>
     </row>
     <row r="1542" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -66117,7 +66133,7 @@
       <c r="T1542" s="7"/>
       <c r="U1542" s="7"/>
       <c r="V1542" s="39" t="s">
-        <v>1434</v>
+        <v>1433</v>
       </c>
     </row>
     <row r="1543" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -66193,7 +66209,7 @@
       <c r="T1544" s="7"/>
       <c r="U1544" s="7"/>
       <c r="V1544" s="51" t="s">
-        <v>1435</v>
+        <v>1434</v>
       </c>
     </row>
     <row r="1545" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -66578,7 +66594,7 @@
       <c r="T1554" s="7"/>
       <c r="U1554" s="7"/>
       <c r="V1554" s="39" t="s">
-        <v>1436</v>
+        <v>1435</v>
       </c>
     </row>
     <row r="1555" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -66626,7 +66642,7 @@
       </c>
       <c r="U1555" s="7"/>
       <c r="V1555" s="39" t="s">
-        <v>1437</v>
+        <v>1436</v>
       </c>
     </row>
     <row r="1556" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -66967,7 +66983,7 @@
       <c r="T1564" s="7"/>
       <c r="U1564" s="7"/>
       <c r="V1564" s="39" t="s">
-        <v>1416</v>
+        <v>1415</v>
       </c>
     </row>
     <row r="1565" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -67010,7 +67026,7 @@
       <c r="T1565" s="7"/>
       <c r="U1565" s="7"/>
       <c r="V1565" s="39" t="s">
-        <v>1438</v>
+        <v>1437</v>
       </c>
     </row>
     <row r="1566" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -67049,7 +67065,7 @@
       <c r="T1566" s="7"/>
       <c r="U1566" s="7"/>
       <c r="V1566" s="39" t="s">
-        <v>1439</v>
+        <v>1438</v>
       </c>
     </row>
     <row r="1567" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -67088,7 +67104,7 @@
       <c r="T1567" s="7"/>
       <c r="U1567" s="7"/>
       <c r="V1567" s="39" t="s">
-        <v>1440</v>
+        <v>1439</v>
       </c>
     </row>
     <row r="1568" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -67164,7 +67180,7 @@
       <c r="T1569" s="7"/>
       <c r="U1569" s="7"/>
       <c r="V1569" s="39" t="s">
-        <v>1441</v>
+        <v>1440</v>
       </c>
     </row>
     <row r="1570" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -67203,7 +67219,7 @@
       <c r="T1570" s="7"/>
       <c r="U1570" s="7"/>
       <c r="V1570" s="39" t="s">
-        <v>1442</v>
+        <v>1441</v>
       </c>
     </row>
     <row r="1571" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -67242,7 +67258,7 @@
       <c r="T1571" s="7"/>
       <c r="U1571" s="7"/>
       <c r="V1571" s="39" t="s">
-        <v>1443</v>
+        <v>1442</v>
       </c>
     </row>
     <row r="1572" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -67318,7 +67334,7 @@
       <c r="T1573" s="7"/>
       <c r="U1573" s="7"/>
       <c r="V1573" s="39" t="s">
-        <v>1442</v>
+        <v>1441</v>
       </c>
     </row>
     <row r="1574" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -67435,7 +67451,7 @@
       <c r="T1576" s="7"/>
       <c r="U1576" s="7"/>
       <c r="V1576" s="39" t="s">
-        <v>1402</v>
+        <v>1401</v>
       </c>
     </row>
     <row r="1577" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -67616,7 +67632,7 @@
         <v>72</v>
       </c>
       <c r="V1581" s="39" t="s">
-        <v>1444</v>
+        <v>1443</v>
       </c>
     </row>
     <row r="1582" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -67828,7 +67844,7 @@
         <v>72</v>
       </c>
       <c r="V1588" s="39" t="s">
-        <v>1445</v>
+        <v>1444</v>
       </c>
     </row>
     <row r="1589" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -67960,7 +67976,7 @@
         <v>72</v>
       </c>
       <c r="V1593" s="39" t="s">
-        <v>1446</v>
+        <v>1445</v>
       </c>
     </row>
     <row r="1594" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -68405,7 +68421,7 @@
         <v>72</v>
       </c>
       <c r="V1610" s="39" t="s">
-        <v>1447</v>
+        <v>1446</v>
       </c>
     </row>
     <row r="1611" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -68434,7 +68450,7 @@
         <v>72</v>
       </c>
       <c r="V1611" s="39" t="s">
-        <v>1448</v>
+        <v>1447</v>
       </c>
     </row>
     <row r="1612" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -68541,7 +68557,7 @@
         <v>72</v>
       </c>
       <c r="V1615" s="39" t="s">
-        <v>1449</v>
+        <v>1448</v>
       </c>
     </row>
     <row r="1616" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -68596,7 +68612,7 @@
         <v>72</v>
       </c>
       <c r="V1617" s="39" t="s">
-        <v>1450</v>
+        <v>1449</v>
       </c>
     </row>
     <row r="1618" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -68677,7 +68693,7 @@
         <v>72</v>
       </c>
       <c r="V1620" s="39" t="s">
-        <v>1451</v>
+        <v>1450</v>
       </c>
     </row>
     <row r="1621" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -68848,7 +68864,7 @@
         <v>72</v>
       </c>
       <c r="V1626" s="39" t="s">
-        <v>1452</v>
+        <v>1451</v>
       </c>
     </row>
     <row r="1627" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -69193,7 +69209,7 @@
         <v>73</v>
       </c>
       <c r="V1638" s="39" t="s">
-        <v>1453</v>
+        <v>1452</v>
       </c>
     </row>
     <row r="1639" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -69443,7 +69459,7 @@
         <v>73</v>
       </c>
       <c r="V1647" s="39" t="s">
-        <v>1454</v>
+        <v>1453</v>
       </c>
     </row>
     <row r="1648" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -69697,7 +69713,7 @@
         <v>73</v>
       </c>
       <c r="V1655" s="39" t="s">
-        <v>1455</v>
+        <v>1454</v>
       </c>
     </row>
     <row r="1656" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -69729,7 +69745,7 @@
         <v>72</v>
       </c>
       <c r="V1656" s="39" t="s">
-        <v>1456</v>
+        <v>1455</v>
       </c>
     </row>
     <row r="1657" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -69851,7 +69867,7 @@
         <v>72</v>
       </c>
       <c r="V1660" s="39" t="s">
-        <v>1457</v>
+        <v>1456</v>
       </c>
     </row>
     <row r="1661" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -69918,7 +69934,7 @@
         <v>82</v>
       </c>
       <c r="V1662" s="39" t="s">
-        <v>1458</v>
+        <v>1457</v>
       </c>
     </row>
     <row r="1663" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -69950,7 +69966,7 @@
         <v>73</v>
       </c>
       <c r="V1663" s="39" t="s">
-        <v>1459</v>
+        <v>1458</v>
       </c>
     </row>
     <row r="1664" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -70040,7 +70056,7 @@
         <v>72</v>
       </c>
       <c r="V1666" s="39" t="s">
-        <v>1460</v>
+        <v>1459</v>
       </c>
     </row>
     <row r="1667" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -70075,7 +70091,7 @@
         <v>72</v>
       </c>
       <c r="V1667" s="39" t="s">
-        <v>1461</v>
+        <v>1460</v>
       </c>
     </row>
     <row r="1668" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -70243,7 +70259,7 @@
       </c>
       <c r="U1672" s="7"/>
       <c r="V1672" s="39" t="s">
-        <v>1462</v>
+        <v>1461</v>
       </c>
     </row>
     <row r="1673" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -70366,7 +70382,7 @@
         <v>72</v>
       </c>
       <c r="V1676" s="39" t="s">
-        <v>1463</v>
+        <v>1462</v>
       </c>
     </row>
     <row r="1677" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -70398,7 +70414,7 @@
         <v>72</v>
       </c>
       <c r="V1677" s="39" t="s">
-        <v>1464</v>
+        <v>1463</v>
       </c>
     </row>
     <row r="1678" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -70488,7 +70504,7 @@
         <v>73</v>
       </c>
       <c r="V1680" s="51" t="s">
-        <v>1465</v>
+        <v>1464</v>
       </c>
     </row>
     <row r="1681" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -70523,7 +70539,7 @@
         <v>74</v>
       </c>
       <c r="V1681" s="39" t="s">
-        <v>1466</v>
+        <v>1465</v>
       </c>
     </row>
     <row r="1682" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -70687,7 +70703,7 @@
         <v>73</v>
       </c>
       <c r="V1686" s="39" t="s">
-        <v>1467</v>
+        <v>1466</v>
       </c>
     </row>
     <row r="1687" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -70856,7 +70872,7 @@
         <v>73</v>
       </c>
       <c r="V1691" s="39" t="s">
-        <v>1468</v>
+        <v>1467</v>
       </c>
     </row>
     <row r="1692" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -70888,7 +70904,7 @@
         <v>72</v>
       </c>
       <c r="V1692" s="39" t="s">
-        <v>1469</v>
+        <v>1468</v>
       </c>
     </row>
     <row r="1693" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -71007,7 +71023,7 @@
         <v>72</v>
       </c>
       <c r="V1696" s="39" t="s">
-        <v>1470</v>
+        <v>1469</v>
       </c>
     </row>
     <row r="1697" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -71039,7 +71055,7 @@
         <v>72</v>
       </c>
       <c r="V1697" s="39" t="s">
-        <v>1471</v>
+        <v>1470</v>
       </c>
     </row>
     <row r="1698" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -71070,7 +71086,7 @@
         <v>73</v>
       </c>
       <c r="V1698" s="39" t="s">
-        <v>1472</v>
+        <v>1471</v>
       </c>
     </row>
     <row r="1699" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -71169,7 +71185,7 @@
         <v>72</v>
       </c>
       <c r="V1701" s="39" t="s">
-        <v>1473</v>
+        <v>1472</v>
       </c>
     </row>
     <row r="1702" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -71291,7 +71307,7 @@
         <v>72</v>
       </c>
       <c r="V1705" s="39" t="s">
-        <v>1474</v>
+        <v>1473</v>
       </c>
     </row>
     <row r="1706" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -71355,7 +71371,7 @@
       </c>
       <c r="U1707" s="7"/>
       <c r="V1707" s="51" t="s">
-        <v>1475</v>
+        <v>1474</v>
       </c>
     </row>
     <row r="1708" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -71476,7 +71492,7 @@
         <v>72</v>
       </c>
       <c r="V1711" s="39" t="s">
-        <v>1456</v>
+        <v>1455</v>
       </c>
     </row>
     <row r="1712" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -71540,7 +71556,7 @@
         <v>73</v>
       </c>
       <c r="V1713" s="39" t="s">
-        <v>1476</v>
+        <v>1475</v>
       </c>
     </row>
     <row r="1714" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -71572,7 +71588,7 @@
         <v>72</v>
       </c>
       <c r="V1714" s="39" t="s">
-        <v>1477</v>
+        <v>1476</v>
       </c>
     </row>
     <row r="1715" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -71610,7 +71626,7 @@
         <v>86</v>
       </c>
       <c r="V1715" s="39" t="s">
-        <v>1478</v>
+        <v>1477</v>
       </c>
     </row>
     <row r="1716" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -71823,7 +71839,7 @@
         <v>73</v>
       </c>
       <c r="V1721" s="39" t="s">
-        <v>1453</v>
+        <v>1452</v>
       </c>
     </row>
     <row r="1722" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -72103,7 +72119,7 @@
         <v>73</v>
       </c>
       <c r="V1730" s="39" t="s">
-        <v>1454</v>
+        <v>1453</v>
       </c>
     </row>
     <row r="1731" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -72164,7 +72180,7 @@
         <v>72</v>
       </c>
       <c r="V1732" s="39" t="s">
-        <v>1479</v>
+        <v>1478</v>
       </c>
     </row>
     <row r="1733" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -72302,7 +72318,7 @@
         <v>73</v>
       </c>
       <c r="V1736" s="39" t="s">
-        <v>1480</v>
+        <v>1479</v>
       </c>
     </row>
     <row r="1737" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -72392,7 +72408,7 @@
         <v>72</v>
       </c>
       <c r="V1739" s="39" t="s">
-        <v>1481</v>
+        <v>1480</v>
       </c>
     </row>
     <row r="1740" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -72427,7 +72443,7 @@
         <v>73</v>
       </c>
       <c r="V1740" s="39" t="s">
-        <v>1482</v>
+        <v>1481</v>
       </c>
     </row>
     <row r="1741" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -72520,7 +72536,7 @@
         <v>72</v>
       </c>
       <c r="V1743" s="39" t="s">
-        <v>1483</v>
+        <v>1482</v>
       </c>
     </row>
     <row r="1744" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -72705,7 +72721,7 @@
         <v>73</v>
       </c>
       <c r="V1749" s="39" t="s">
-        <v>1484</v>
+        <v>1483</v>
       </c>
     </row>
     <row r="1750" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -72795,7 +72811,7 @@
         <v>72</v>
       </c>
       <c r="V1752" s="39" t="s">
-        <v>1485</v>
+        <v>1484</v>
       </c>
     </row>
     <row r="1753" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -72952,7 +72968,7 @@
         <v>73</v>
       </c>
       <c r="V1757" s="39" t="s">
-        <v>1486</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="1758" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -73051,7 +73067,7 @@
         <v>72</v>
       </c>
       <c r="V1760" s="39" t="s">
-        <v>1487</v>
+        <v>1486</v>
       </c>
     </row>
     <row r="1761" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -73144,7 +73160,7 @@
         <v>73</v>
       </c>
       <c r="V1763" s="40" t="s">
-        <v>1488</v>
+        <v>1487</v>
       </c>
     </row>
     <row r="1764" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -73266,7 +73282,7 @@
         <v>73</v>
       </c>
       <c r="V1767" s="39" t="s">
-        <v>1489</v>
+        <v>1488</v>
       </c>
     </row>
     <row r="1768" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -73595,7 +73611,7 @@
         <v>73</v>
       </c>
       <c r="V1777" s="39" t="s">
-        <v>1490</v>
+        <v>1489</v>
       </c>
     </row>
     <row r="1778" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -73833,7 +73849,7 @@
         <v>73</v>
       </c>
       <c r="V1785" s="39" t="s">
-        <v>1491</v>
+        <v>1490</v>
       </c>
     </row>
     <row r="1786" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -74014,7 +74030,7 @@
         <v>72</v>
       </c>
       <c r="V1791" s="40" t="s">
-        <v>1492</v>
+        <v>1491</v>
       </c>
     </row>
     <row r="1792" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -74046,7 +74062,7 @@
         <v>73</v>
       </c>
       <c r="V1792" s="39" t="s">
-        <v>1493</v>
+        <v>1492</v>
       </c>
     </row>
     <row r="1793" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -74078,7 +74094,7 @@
         <v>72</v>
       </c>
       <c r="V1793" s="39" t="s">
-        <v>1494</v>
+        <v>1493</v>
       </c>
     </row>
     <row r="1794" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -74113,7 +74129,7 @@
         <v>73</v>
       </c>
       <c r="V1794" s="39" t="s">
-        <v>1495</v>
+        <v>1494</v>
       </c>
     </row>
     <row r="1795" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -74354,7 +74370,7 @@
         <v>73</v>
       </c>
       <c r="V1802" s="39" t="s">
-        <v>1496</v>
+        <v>1495</v>
       </c>
     </row>
     <row r="1803" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -74447,7 +74463,7 @@
         <v>73</v>
       </c>
       <c r="V1805" s="39" t="s">
-        <v>1497</v>
+        <v>1496</v>
       </c>
     </row>
     <row r="1806" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -74648,7 +74664,7 @@
         <v>73</v>
       </c>
       <c r="V1811" s="39" t="s">
-        <v>1498</v>
+        <v>1497</v>
       </c>
     </row>
     <row r="1812" spans="3:22" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
TS PP 1.1 - 1.8 Final 17/10/2021
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Padam Input Templates/TS 1.4 Padam Input Template.xlsx
+++ b/TS Jatai Working/Padam Input Templates/TS 1.4 Padam Input Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\texts\TS Jatai Working\Padam Input Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2019ED23-ECA7-4AD2-B406-D5A3F36611A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B61B23E2-08F1-45F8-A303-DFDE1FC3654E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4730,7 +4730,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -4930,9 +4930,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -5220,10 +5217,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V1812"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="O1402" sqref="O1402"/>
+      <selection pane="bottomLeft" activeCell="T6" sqref="T6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -32651,7 +32648,7 @@
       <c r="N674" s="39" t="s">
         <v>521</v>
       </c>
-      <c r="O674" s="71" t="s">
+      <c r="O674" s="70" t="s">
         <v>72</v>
       </c>
       <c r="P674" s="7"/>
@@ -39693,7 +39690,7 @@
       <c r="N859" s="39" t="s">
         <v>624</v>
       </c>
-      <c r="O859" s="71" t="s">
+      <c r="O859" s="70" t="s">
         <v>74</v>
       </c>
       <c r="P859" s="7"/>
@@ -43624,7 +43621,7 @@
       <c r="S963" s="7"/>
       <c r="T963" s="7"/>
       <c r="U963" s="7"/>
-      <c r="V963" s="70"/>
+      <c r="V963" s="51"/>
     </row>
     <row r="964" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="E964" s="18"/>
@@ -48691,7 +48688,7 @@
       <c r="N1096" s="39" t="s">
         <v>747</v>
       </c>
-      <c r="O1096" s="71" t="s">
+      <c r="O1096" s="70" t="s">
         <v>74</v>
       </c>
       <c r="P1096" s="7"/>
@@ -52539,7 +52536,7 @@
       <c r="N1198" s="39" t="s">
         <v>783</v>
       </c>
-      <c r="O1198" s="71" t="s">
+      <c r="O1198" s="70" t="s">
         <v>72</v>
       </c>
       <c r="P1198" s="7"/>
@@ -60487,7 +60484,7 @@
       <c r="N1402" s="51" t="s">
         <v>903</v>
       </c>
-      <c r="O1402" s="71" t="s">
+      <c r="O1402" s="70" t="s">
         <v>72</v>
       </c>
       <c r="P1402" s="7"/>

</xml_diff>

<commit_message>
TS 1.4 Ghanam files Tamil - 08/11/2021
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Padam Input Templates/TS 1.4 Padam Input Template.xlsx
+++ b/TS Jatai Working/Padam Input Templates/TS 1.4 Padam Input Template.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Documents\GitHub\texts\TS Jatai Working\Padam Input Templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\texts\TS Jatai Working\Padam Input Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEDA679C-A8C1-4416-BE7D-60F2CB8E01E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TS 1.4" sheetId="1" r:id="rId1"/>
@@ -17,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'TS 1.4'!$C$1:$V$1811</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -4536,7 +4537,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -4679,7 +4680,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -4701,6 +4702,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4732,7 +4739,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -4938,6 +4945,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -5219,13 +5229,13 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V1812"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1694" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A965" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="V1698" sqref="V1698"/>
+      <selection pane="bottomLeft" activeCell="O971" sqref="O971"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -43930,10 +43940,10 @@
       <c r="P971" s="7"/>
       <c r="Q971" s="7"/>
       <c r="R971" s="7"/>
-      <c r="S971" s="7" t="s">
+      <c r="S971" s="72" t="s">
         <v>80</v>
       </c>
-      <c r="T971" s="7" t="s">
+      <c r="T971" s="72" t="s">
         <v>85</v>
       </c>
       <c r="U971" s="7"/>

</xml_diff>

<commit_message>
TS 1.4 Tamil Ghanam and Jatai files - 09/11/2021
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Padam Input Templates/TS 1.4 Padam Input Template.xlsx
+++ b/TS Jatai Working/Padam Input Templates/TS 1.4 Padam Input Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\texts\TS Jatai Working\Padam Input Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEDA679C-A8C1-4416-BE7D-60F2CB8E01E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5025A3C-448B-400D-8337-A40D8A6EDF8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6745" uniqueCount="1499">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6745" uniqueCount="1500">
   <si>
     <t>Passage</t>
   </si>
@@ -4532,6 +4532,9 @@
   </si>
   <si>
     <t>suqtAsaq iti# suqtAsa#H</t>
+  </si>
+  <si>
+    <t>N[Sh]</t>
   </si>
 </sst>
 </file>
@@ -4680,7 +4683,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -4702,12 +4705,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4947,7 +4944,7 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -5233,9 +5230,9 @@
   <dimension ref="A1:V1812"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A965" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="O971" sqref="O971"/>
+      <selection pane="bottomLeft" activeCell="S971" sqref="S971:T971"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -43941,10 +43938,10 @@
       <c r="Q971" s="7"/>
       <c r="R971" s="7"/>
       <c r="S971" s="72" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="T971" s="72" t="s">
-        <v>85</v>
+        <v>1499</v>
       </c>
       <c r="U971" s="7"/>
       <c r="V971" s="39" t="s">

</xml_diff>

<commit_message>
nmv 10 02 2023
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Padam Input Templates/TS 1.4 Padam Input Template.xlsx
+++ b/TS Jatai Working/Padam Input Templates/TS 1.4 Padam Input Template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALL IMP DATA\GitHub\texts\TS Jatai Working\Padam Input Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8BD35E0-3BE3-46A0-AFEE-9ED8577FBB15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0051A71C-7171-45EA-9748-CC61ED98A925}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,20 +23,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6784" uniqueCount="1498">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6750" uniqueCount="1497">
   <si>
     <t>Passage</t>
   </si>
@@ -3671,9 +3663,6 @@
     <t>riqhaqntIti# rihanti</t>
   </si>
   <si>
-    <t>uqpaqyAqmagRu#hItaq ityu#payAqma - gRuhIqtaqH</t>
-  </si>
-  <si>
     <t>pAqhIti# pAhi</t>
   </si>
   <si>
@@ -3831,9 +3820,6 @@
   </si>
   <si>
     <t>kaqrtRuBiqriti# kaqrtRu - BiqH</t>
-  </si>
-  <si>
-    <t>Buqditi# BUt</t>
   </si>
   <si>
     <t>dAqSuShaq iti# dAqSuShe$</t>
@@ -4669,6 +4655,9 @@
       </rPr>
       <t>viveSa</t>
     </r>
+  </si>
+  <si>
+    <t>BUqditi# BUt</t>
   </si>
 </sst>
 </file>
@@ -5354,9 +5343,9 @@
   <dimension ref="A1:V1812"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="O1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1529" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A689" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="V1536" sqref="V1536"/>
+      <selection pane="bottomLeft" activeCell="V695" sqref="V695"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -18290,8 +18279,8 @@
       <c r="S331" s="7"/>
       <c r="T331" s="7"/>
       <c r="U331" s="7"/>
-      <c r="V331" s="33" t="s">
-        <v>1211</v>
+      <c r="V331" s="34" t="s">
+        <v>1174</v>
       </c>
     </row>
     <row r="332" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -18573,7 +18562,7 @@
       <c r="T339" s="7"/>
       <c r="U339" s="7"/>
       <c r="V339" s="33" t="s">
-        <v>1212</v>
+        <v>1211</v>
       </c>
     </row>
     <row r="340" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -18783,7 +18772,7 @@
       <c r="T345" s="7"/>
       <c r="U345" s="7"/>
       <c r="V345" s="33" t="s">
-        <v>1213</v>
+        <v>1212</v>
       </c>
     </row>
     <row r="346" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -18820,7 +18809,7 @@
       <c r="T346" s="7"/>
       <c r="U346" s="7"/>
       <c r="V346" s="33" t="s">
-        <v>1214</v>
+        <v>1213</v>
       </c>
     </row>
     <row r="347" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -18857,7 +18846,7 @@
       <c r="T347" s="7"/>
       <c r="U347" s="7"/>
       <c r="V347" s="33" t="s">
-        <v>1215</v>
+        <v>1214</v>
       </c>
     </row>
     <row r="348" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -19178,7 +19167,7 @@
       <c r="T356" s="7"/>
       <c r="U356" s="7"/>
       <c r="V356" s="33" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
     </row>
     <row r="357" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -19470,7 +19459,7 @@
       <c r="T364" s="7"/>
       <c r="U364" s="7"/>
       <c r="V364" s="33" t="s">
-        <v>1217</v>
+        <v>1216</v>
       </c>
     </row>
     <row r="365" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -19508,7 +19497,7 @@
       <c r="T365" s="7"/>
       <c r="U365" s="7"/>
       <c r="V365" s="33" t="s">
-        <v>1212</v>
+        <v>1211</v>
       </c>
     </row>
     <row r="366" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -19876,7 +19865,7 @@
       <c r="T375" s="7"/>
       <c r="U375" s="7"/>
       <c r="V375" s="33" t="s">
-        <v>1218</v>
+        <v>1217</v>
       </c>
     </row>
     <row r="376" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -20335,7 +20324,7 @@
       <c r="T388" s="7"/>
       <c r="U388" s="7"/>
       <c r="V388" s="33" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
     </row>
     <row r="389" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -20477,7 +20466,7 @@
       <c r="T392" s="7"/>
       <c r="U392" s="7"/>
       <c r="V392" s="33" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
     </row>
     <row r="393" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -21041,7 +21030,7 @@
       <c r="T408" s="7"/>
       <c r="U408" s="7"/>
       <c r="V408" s="33" t="s">
-        <v>1221</v>
+        <v>1220</v>
       </c>
     </row>
     <row r="409" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -21391,7 +21380,7 @@
       <c r="T418" s="7"/>
       <c r="U418" s="7"/>
       <c r="V418" s="33" t="s">
-        <v>1222</v>
+        <v>1221</v>
       </c>
     </row>
     <row r="419" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -21465,7 +21454,7 @@
         <v>81</v>
       </c>
       <c r="V420" s="33" t="s">
-        <v>1218</v>
+        <v>1217</v>
       </c>
     </row>
     <row r="421" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -21642,7 +21631,7 @@
       <c r="T425" s="7"/>
       <c r="U425" s="7"/>
       <c r="V425" s="33" t="s">
-        <v>1223</v>
+        <v>1222</v>
       </c>
     </row>
     <row r="426" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -21821,7 +21810,7 @@
       <c r="T430" s="7"/>
       <c r="U430" s="7"/>
       <c r="V430" s="33" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
     </row>
     <row r="431" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -21963,7 +21952,7 @@
       <c r="T434" s="7"/>
       <c r="U434" s="7"/>
       <c r="V434" s="33" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
     </row>
     <row r="435" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -22529,7 +22518,7 @@
       <c r="T450" s="7"/>
       <c r="U450" s="7"/>
       <c r="V450" s="33" t="s">
-        <v>1221</v>
+        <v>1220</v>
       </c>
     </row>
     <row r="451" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -22706,7 +22695,7 @@
       <c r="T455" s="7"/>
       <c r="U455" s="7"/>
       <c r="V455" s="33" t="s">
-        <v>1224</v>
+        <v>1223</v>
       </c>
     </row>
     <row r="456" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -22778,7 +22767,7 @@
       <c r="T457" s="7"/>
       <c r="U457" s="7"/>
       <c r="V457" s="33" t="s">
-        <v>1225</v>
+        <v>1224</v>
       </c>
     </row>
     <row r="458" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -23315,7 +23304,7 @@
       <c r="T472" s="7"/>
       <c r="U472" s="7"/>
       <c r="V472" s="33" t="s">
-        <v>1225</v>
+        <v>1224</v>
       </c>
     </row>
     <row r="473" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -23597,7 +23586,7 @@
       <c r="T480" s="7"/>
       <c r="U480" s="7"/>
       <c r="V480" s="33" t="s">
-        <v>1226</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="481" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -23669,7 +23658,7 @@
       <c r="T482" s="7"/>
       <c r="U482" s="7"/>
       <c r="V482" s="33" t="s">
-        <v>1227</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="483" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -23931,7 +23920,7 @@
       <c r="T489" s="7"/>
       <c r="U489" s="7"/>
       <c r="V489" s="33" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="490" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -24215,7 +24204,7 @@
       <c r="T497" s="7"/>
       <c r="U497" s="7"/>
       <c r="V497" s="33" t="s">
-        <v>1229</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="498" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -24287,7 +24276,7 @@
       <c r="T499" s="7"/>
       <c r="U499" s="7"/>
       <c r="V499" s="33" t="s">
-        <v>1230</v>
+        <v>1229</v>
       </c>
     </row>
     <row r="500" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -24365,7 +24354,7 @@
       <c r="T501" s="7"/>
       <c r="U501" s="7"/>
       <c r="V501" s="33" t="s">
-        <v>1231</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="502" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -24580,7 +24569,7 @@
       <c r="T507" s="7"/>
       <c r="U507" s="7"/>
       <c r="V507" s="33" t="s">
-        <v>1232</v>
+        <v>1231</v>
       </c>
     </row>
     <row r="508" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -25530,7 +25519,7 @@
       <c r="T534" s="7"/>
       <c r="U534" s="7"/>
       <c r="V534" s="33" t="s">
-        <v>1233</v>
+        <v>1232</v>
       </c>
     </row>
     <row r="535" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -25608,7 +25597,7 @@
       <c r="T536" s="7"/>
       <c r="U536" s="7"/>
       <c r="V536" s="33" t="s">
-        <v>1234</v>
+        <v>1233</v>
       </c>
     </row>
     <row r="537" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -25686,7 +25675,7 @@
       <c r="T538" s="7"/>
       <c r="U538" s="7"/>
       <c r="V538" s="33" t="s">
-        <v>1235</v>
+        <v>1234</v>
       </c>
     </row>
     <row r="539" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -25915,7 +25904,7 @@
       <c r="T544" s="7"/>
       <c r="U544" s="7"/>
       <c r="V544" s="33" t="s">
-        <v>1236</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="545" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -26057,7 +26046,7 @@
       <c r="T548" s="7"/>
       <c r="U548" s="7"/>
       <c r="V548" s="33" t="s">
-        <v>1237</v>
+        <v>1236</v>
       </c>
     </row>
     <row r="549" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -26166,7 +26155,7 @@
       <c r="T551" s="7"/>
       <c r="U551" s="7"/>
       <c r="V551" s="33" t="s">
-        <v>1238</v>
+        <v>1237</v>
       </c>
     </row>
     <row r="552" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -26343,7 +26332,7 @@
       <c r="T556" s="7"/>
       <c r="U556" s="7"/>
       <c r="V556" s="33" t="s">
-        <v>1238</v>
+        <v>1237</v>
       </c>
     </row>
     <row r="557" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -26453,7 +26442,7 @@
       <c r="T559" s="7"/>
       <c r="U559" s="7"/>
       <c r="V559" s="33" t="s">
-        <v>1239</v>
+        <v>1238</v>
       </c>
     </row>
     <row r="560" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -26598,7 +26587,7 @@
       <c r="T563" s="7"/>
       <c r="U563" s="7"/>
       <c r="V563" s="33" t="s">
-        <v>1240</v>
+        <v>1239</v>
       </c>
     </row>
     <row r="564" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -26705,7 +26694,7 @@
       <c r="T566" s="7"/>
       <c r="U566" s="7"/>
       <c r="V566" s="33" t="s">
-        <v>1241</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="567" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -27096,7 +27085,7 @@
       <c r="T577" s="7"/>
       <c r="U577" s="7"/>
       <c r="V577" s="33" t="s">
-        <v>1221</v>
+        <v>1220</v>
       </c>
     </row>
     <row r="578" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -27236,7 +27225,7 @@
       <c r="T581" s="7"/>
       <c r="U581" s="7"/>
       <c r="V581" s="33" t="s">
-        <v>1242</v>
+        <v>1241</v>
       </c>
     </row>
     <row r="582" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -27343,7 +27332,7 @@
       <c r="T584" s="7"/>
       <c r="U584" s="7"/>
       <c r="V584" s="33" t="s">
-        <v>1243</v>
+        <v>1242</v>
       </c>
     </row>
     <row r="585" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -27380,7 +27369,7 @@
       <c r="T585" s="7"/>
       <c r="U585" s="7"/>
       <c r="V585" s="33" t="s">
-        <v>1244</v>
+        <v>1243</v>
       </c>
     </row>
     <row r="586" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -27522,7 +27511,7 @@
       <c r="T589" s="7"/>
       <c r="U589" s="7"/>
       <c r="V589" s="33" t="s">
-        <v>1245</v>
+        <v>1244</v>
       </c>
     </row>
     <row r="590" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -27629,7 +27618,7 @@
       <c r="T592" s="7"/>
       <c r="U592" s="7"/>
       <c r="V592" s="33" t="s">
-        <v>1246</v>
+        <v>1245</v>
       </c>
     </row>
     <row r="593" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -28337,7 +28326,7 @@
       <c r="T612" s="7"/>
       <c r="U612" s="7"/>
       <c r="V612" s="33" t="s">
-        <v>1247</v>
+        <v>1246</v>
       </c>
     </row>
     <row r="613" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -28411,7 +28400,7 @@
       <c r="T614" s="7"/>
       <c r="U614" s="7"/>
       <c r="V614" s="33" t="s">
-        <v>1248</v>
+        <v>1247</v>
       </c>
     </row>
     <row r="615" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -28662,7 +28651,7 @@
       <c r="T621" s="7"/>
       <c r="U621" s="7"/>
       <c r="V621" s="33" t="s">
-        <v>1249</v>
+        <v>1248</v>
       </c>
     </row>
     <row r="622" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -29303,7 +29292,7 @@
       <c r="T639" s="7"/>
       <c r="U639" s="7"/>
       <c r="V639" s="33" t="s">
-        <v>1250</v>
+        <v>1249</v>
       </c>
     </row>
     <row r="640" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -29340,7 +29329,7 @@
       <c r="T640" s="7"/>
       <c r="U640" s="7"/>
       <c r="V640" s="33" t="s">
-        <v>1251</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="641" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -29661,7 +29650,7 @@
       <c r="T649" s="7"/>
       <c r="U649" s="7"/>
       <c r="V649" s="33" t="s">
-        <v>1252</v>
+        <v>1251</v>
       </c>
     </row>
     <row r="650" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -29699,7 +29688,7 @@
       <c r="T650" s="7"/>
       <c r="U650" s="7"/>
       <c r="V650" s="33" t="s">
-        <v>1253</v>
+        <v>1252</v>
       </c>
     </row>
     <row r="651" spans="1:22" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -30309,7 +30298,7 @@
       </c>
       <c r="U667" s="7"/>
       <c r="V667" s="33" t="s">
-        <v>1254</v>
+        <v>1253</v>
       </c>
     </row>
     <row r="668" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -30344,7 +30333,7 @@
       <c r="T668" s="7"/>
       <c r="U668" s="7"/>
       <c r="V668" s="33" t="s">
-        <v>1255</v>
+        <v>1254</v>
       </c>
     </row>
     <row r="669" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -30445,7 +30434,7 @@
       <c r="T671" s="7"/>
       <c r="U671" s="7"/>
       <c r="V671" s="33" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
     </row>
     <row r="672" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -30548,7 +30537,7 @@
       <c r="T674" s="7"/>
       <c r="U674" s="7"/>
       <c r="V674" s="33" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
     </row>
     <row r="675" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -30715,7 +30704,7 @@
       <c r="T679" s="7"/>
       <c r="U679" s="7"/>
       <c r="V679" s="33" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
     </row>
     <row r="680" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -30853,7 +30842,7 @@
       <c r="T683" s="7"/>
       <c r="U683" s="7"/>
       <c r="V683" s="33" t="s">
-        <v>1258</v>
+        <v>1257</v>
       </c>
     </row>
     <row r="684" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -30923,7 +30912,7 @@
       <c r="T685" s="7"/>
       <c r="U685" s="7"/>
       <c r="V685" s="33" t="s">
-        <v>1259</v>
+        <v>1258</v>
       </c>
     </row>
     <row r="686" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -30991,7 +30980,7 @@
       <c r="T687" s="7"/>
       <c r="U687" s="7"/>
       <c r="V687" s="33" t="s">
-        <v>1260</v>
+        <v>1259</v>
       </c>
     </row>
     <row r="688" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -31061,7 +31050,7 @@
       <c r="T689" s="7"/>
       <c r="U689" s="7"/>
       <c r="V689" s="33" t="s">
-        <v>1261</v>
+        <v>1260</v>
       </c>
     </row>
     <row r="690" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -31096,7 +31085,7 @@
       <c r="T690" s="7"/>
       <c r="U690" s="7"/>
       <c r="V690" s="33" t="s">
-        <v>1262</v>
+        <v>1261</v>
       </c>
     </row>
     <row r="691" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -31263,7 +31252,7 @@
       <c r="T695" s="7"/>
       <c r="U695" s="7"/>
       <c r="V695" s="33" t="s">
-        <v>1263</v>
+        <v>1262</v>
       </c>
     </row>
     <row r="696" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -31298,7 +31287,7 @@
       <c r="T696" s="7"/>
       <c r="U696" s="7"/>
       <c r="V696" s="33" t="s">
-        <v>1264</v>
+        <v>1263</v>
       </c>
     </row>
     <row r="697" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -31332,8 +31321,8 @@
       <c r="S697" s="7"/>
       <c r="T697" s="7"/>
       <c r="U697" s="7"/>
-      <c r="V697" s="33" t="s">
-        <v>1265</v>
+      <c r="V697" s="34" t="s">
+        <v>1496</v>
       </c>
     </row>
     <row r="698" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -31436,7 +31425,7 @@
       <c r="T700" s="7"/>
       <c r="U700" s="7"/>
       <c r="V700" s="33" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
     </row>
     <row r="701" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -31603,7 +31592,7 @@
       <c r="T705" s="7"/>
       <c r="U705" s="7"/>
       <c r="V705" s="33" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
     </row>
     <row r="706" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -31914,7 +31903,7 @@
       <c r="T714" s="7"/>
       <c r="U714" s="7"/>
       <c r="V714" s="33" t="s">
-        <v>1266</v>
+        <v>1264</v>
       </c>
     </row>
     <row r="715" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -31952,7 +31941,7 @@
       <c r="T715" s="7"/>
       <c r="U715" s="7"/>
       <c r="V715" s="33" t="s">
-        <v>1267</v>
+        <v>1265</v>
       </c>
     </row>
     <row r="716" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -32062,7 +32051,7 @@
       <c r="T718" s="7"/>
       <c r="U718" s="7"/>
       <c r="V718" s="33" t="s">
-        <v>1268</v>
+        <v>1266</v>
       </c>
     </row>
     <row r="719" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -32295,7 +32284,7 @@
       <c r="T725" s="7"/>
       <c r="U725" s="7"/>
       <c r="V725" s="33" t="s">
-        <v>1269</v>
+        <v>1267</v>
       </c>
     </row>
     <row r="726" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -32605,7 +32594,7 @@
       <c r="T734" s="7"/>
       <c r="U734" s="7"/>
       <c r="V734" s="33" t="s">
-        <v>1270</v>
+        <v>1268</v>
       </c>
     </row>
     <row r="735" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -32711,7 +32700,7 @@
       <c r="T737" s="7"/>
       <c r="U737" s="7"/>
       <c r="V737" s="33" t="s">
-        <v>1271</v>
+        <v>1269</v>
       </c>
     </row>
     <row r="738" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -33012,7 +33001,7 @@
       <c r="T746" s="7"/>
       <c r="U746" s="7"/>
       <c r="V746" s="33" t="s">
-        <v>1272</v>
+        <v>1270</v>
       </c>
     </row>
     <row r="747" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -33291,7 +33280,7 @@
       <c r="T754" s="7"/>
       <c r="U754" s="7"/>
       <c r="V754" s="33" t="s">
-        <v>1273</v>
+        <v>1271</v>
       </c>
     </row>
     <row r="755" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -33424,7 +33413,7 @@
         <v>52</v>
       </c>
       <c r="N758" s="34" t="s">
-        <v>1490</v>
+        <v>1488</v>
       </c>
       <c r="O758" s="6" t="s">
         <v>72</v>
@@ -33436,7 +33425,7 @@
       <c r="T758" s="7"/>
       <c r="U758" s="7"/>
       <c r="V758" s="33" t="s">
-        <v>1274</v>
+        <v>1272</v>
       </c>
     </row>
     <row r="759" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -33607,7 +33596,7 @@
       <c r="T763" s="7"/>
       <c r="U763" s="7"/>
       <c r="V763" s="33" t="s">
-        <v>1275</v>
+        <v>1273</v>
       </c>
     </row>
     <row r="764" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -33643,7 +33632,7 @@
       <c r="T764" s="7"/>
       <c r="U764" s="7"/>
       <c r="V764" s="33" t="s">
-        <v>1276</v>
+        <v>1274</v>
       </c>
     </row>
     <row r="765" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -33811,7 +33800,7 @@
       <c r="T769" s="7"/>
       <c r="U769" s="7"/>
       <c r="V769" s="33" t="s">
-        <v>1277</v>
+        <v>1275</v>
       </c>
     </row>
     <row r="770" spans="6:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -34277,7 +34266,7 @@
       <c r="T783" s="7"/>
       <c r="U783" s="7"/>
       <c r="V783" s="33" t="s">
-        <v>1278</v>
+        <v>1276</v>
       </c>
     </row>
     <row r="784" spans="6:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -34524,7 +34513,7 @@
       <c r="T790" s="7"/>
       <c r="U790" s="7"/>
       <c r="V790" s="33" t="s">
-        <v>1279</v>
+        <v>1277</v>
       </c>
     </row>
     <row r="791" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -34595,7 +34584,7 @@
       <c r="T792" s="7"/>
       <c r="U792" s="7"/>
       <c r="V792" s="33" t="s">
-        <v>1280</v>
+        <v>1278</v>
       </c>
     </row>
     <row r="793" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -34630,7 +34619,7 @@
       <c r="T793" s="7"/>
       <c r="U793" s="7"/>
       <c r="V793" s="33" t="s">
-        <v>1281</v>
+        <v>1279</v>
       </c>
     </row>
     <row r="794" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -34909,7 +34898,7 @@
       <c r="T801" s="7"/>
       <c r="U801" s="7"/>
       <c r="V801" s="33" t="s">
-        <v>1282</v>
+        <v>1280</v>
       </c>
     </row>
     <row r="802" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -34946,7 +34935,7 @@
       <c r="T802" s="7"/>
       <c r="U802" s="7"/>
       <c r="V802" s="33" t="s">
-        <v>1283</v>
+        <v>1281</v>
       </c>
     </row>
     <row r="803" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -35116,7 +35105,7 @@
       <c r="T807" s="7"/>
       <c r="U807" s="7"/>
       <c r="V807" s="34" t="s">
-        <v>1491</v>
+        <v>1489</v>
       </c>
     </row>
     <row r="808" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -35223,7 +35212,7 @@
       </c>
       <c r="U810" s="7"/>
       <c r="V810" s="33" t="s">
-        <v>1284</v>
+        <v>1282</v>
       </c>
     </row>
     <row r="811" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -35493,7 +35482,7 @@
       <c r="T818" s="7"/>
       <c r="U818" s="7"/>
       <c r="V818" s="33" t="s">
-        <v>1285</v>
+        <v>1283</v>
       </c>
     </row>
     <row r="819" spans="6:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -35715,7 +35704,7 @@
         <v>81</v>
       </c>
       <c r="V824" s="33" t="s">
-        <v>1286</v>
+        <v>1284</v>
       </c>
     </row>
     <row r="825" spans="6:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -35750,7 +35739,7 @@
       <c r="T825" s="7"/>
       <c r="U825" s="7"/>
       <c r="V825" s="33" t="s">
-        <v>1287</v>
+        <v>1285</v>
       </c>
     </row>
     <row r="826" spans="6:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -35919,7 +35908,7 @@
       <c r="T830" s="7"/>
       <c r="U830" s="7"/>
       <c r="V830" s="34" t="s">
-        <v>1486</v>
+        <v>1484</v>
       </c>
     </row>
     <row r="831" spans="6:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -35952,7 +35941,7 @@
       <c r="T831" s="7"/>
       <c r="U831" s="7"/>
       <c r="V831" s="33" t="s">
-        <v>1288</v>
+        <v>1286</v>
       </c>
     </row>
     <row r="832" spans="6:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -36088,7 +36077,7 @@
       <c r="T835" s="7"/>
       <c r="U835" s="7"/>
       <c r="V835" s="33" t="s">
-        <v>1289</v>
+        <v>1287</v>
       </c>
     </row>
     <row r="836" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -36222,7 +36211,7 @@
       <c r="T839" s="7"/>
       <c r="U839" s="7"/>
       <c r="V839" s="33" t="s">
-        <v>1290</v>
+        <v>1288</v>
       </c>
     </row>
     <row r="840" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -36391,7 +36380,7 @@
       <c r="T844" s="7"/>
       <c r="U844" s="7"/>
       <c r="V844" s="34" t="s">
-        <v>1491</v>
+        <v>1489</v>
       </c>
     </row>
     <row r="845" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -36424,7 +36413,7 @@
       <c r="T845" s="7"/>
       <c r="U845" s="7"/>
       <c r="V845" s="33" t="s">
-        <v>1291</v>
+        <v>1289</v>
       </c>
     </row>
     <row r="846" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -36495,7 +36484,7 @@
       <c r="T847" s="7"/>
       <c r="U847" s="7"/>
       <c r="V847" s="33" t="s">
-        <v>1292</v>
+        <v>1290</v>
       </c>
     </row>
     <row r="848" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -36797,7 +36786,7 @@
       <c r="T856" s="7"/>
       <c r="U856" s="7"/>
       <c r="V856" s="33" t="s">
-        <v>1221</v>
+        <v>1220</v>
       </c>
     </row>
     <row r="857" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -36830,7 +36819,7 @@
       <c r="T857" s="7"/>
       <c r="U857" s="7"/>
       <c r="V857" s="33" t="s">
-        <v>1293</v>
+        <v>1291</v>
       </c>
     </row>
     <row r="858" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -36898,7 +36887,7 @@
       <c r="T859" s="7"/>
       <c r="U859" s="7"/>
       <c r="V859" s="33" t="s">
-        <v>1294</v>
+        <v>1292</v>
       </c>
     </row>
     <row r="860" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -36933,7 +36922,7 @@
       <c r="T860" s="7"/>
       <c r="U860" s="7"/>
       <c r="V860" s="33" t="s">
-        <v>1295</v>
+        <v>1293</v>
       </c>
     </row>
     <row r="861" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -36968,7 +36957,7 @@
       <c r="T861" s="7"/>
       <c r="U861" s="7"/>
       <c r="V861" s="33" t="s">
-        <v>1296</v>
+        <v>1294</v>
       </c>
     </row>
     <row r="862" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -37097,7 +37086,7 @@
         <v>9</v>
       </c>
       <c r="N865" s="34" t="s">
-        <v>1492</v>
+        <v>1490</v>
       </c>
       <c r="O865" s="6" t="s">
         <v>72</v>
@@ -37109,7 +37098,7 @@
       <c r="T865" s="7"/>
       <c r="U865" s="7"/>
       <c r="V865" s="33" t="s">
-        <v>1297</v>
+        <v>1295</v>
       </c>
     </row>
     <row r="866" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -37144,7 +37133,7 @@
       <c r="T866" s="7"/>
       <c r="U866" s="7"/>
       <c r="V866" s="33" t="s">
-        <v>1298</v>
+        <v>1296</v>
       </c>
     </row>
     <row r="867" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -37410,7 +37399,7 @@
       <c r="T874" s="7"/>
       <c r="U874" s="7"/>
       <c r="V874" s="33" t="s">
-        <v>1299</v>
+        <v>1297</v>
       </c>
     </row>
     <row r="875" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -37776,7 +37765,7 @@
       <c r="T885" s="7"/>
       <c r="U885" s="7"/>
       <c r="V885" s="33" t="s">
-        <v>1300</v>
+        <v>1298</v>
       </c>
     </row>
     <row r="886" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -37811,7 +37800,7 @@
       <c r="T886" s="7"/>
       <c r="U886" s="7"/>
       <c r="V886" s="33" t="s">
-        <v>1301</v>
+        <v>1299</v>
       </c>
     </row>
     <row r="887" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -37846,7 +37835,7 @@
       <c r="T887" s="7"/>
       <c r="U887" s="7"/>
       <c r="V887" s="33" t="s">
-        <v>1302</v>
+        <v>1300</v>
       </c>
     </row>
     <row r="888" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -37881,7 +37870,7 @@
       <c r="T888" s="7"/>
       <c r="U888" s="7"/>
       <c r="V888" s="33" t="s">
-        <v>1303</v>
+        <v>1301</v>
       </c>
     </row>
     <row r="889" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -38114,7 +38103,7 @@
       <c r="T895" s="7"/>
       <c r="U895" s="7"/>
       <c r="V895" s="33" t="s">
-        <v>1304</v>
+        <v>1302</v>
       </c>
     </row>
     <row r="896" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -38486,7 +38475,7 @@
       <c r="T906" s="7"/>
       <c r="U906" s="7"/>
       <c r="V906" s="33" t="s">
-        <v>1305</v>
+        <v>1303</v>
       </c>
     </row>
     <row r="907" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -38590,7 +38579,7 @@
       <c r="T909" s="7"/>
       <c r="U909" s="7"/>
       <c r="V909" s="33" t="s">
-        <v>1306</v>
+        <v>1304</v>
       </c>
     </row>
     <row r="910" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -38962,7 +38951,7 @@
       <c r="T920" s="7"/>
       <c r="U920" s="7"/>
       <c r="V920" s="33" t="s">
-        <v>1307</v>
+        <v>1305</v>
       </c>
     </row>
     <row r="921" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -38998,7 +38987,7 @@
       <c r="T921" s="7"/>
       <c r="U921" s="7"/>
       <c r="V921" s="33" t="s">
-        <v>1308</v>
+        <v>1306</v>
       </c>
     </row>
     <row r="922" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -39144,7 +39133,7 @@
       <c r="T925" s="7"/>
       <c r="U925" s="7"/>
       <c r="V925" s="33" t="s">
-        <v>1309</v>
+        <v>1307</v>
       </c>
     </row>
     <row r="926" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -39184,7 +39173,7 @@
         <v>81</v>
       </c>
       <c r="V926" s="33" t="s">
-        <v>1310</v>
+        <v>1308</v>
       </c>
     </row>
     <row r="927" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -39285,7 +39274,7 @@
       <c r="T929" s="7"/>
       <c r="U929" s="7"/>
       <c r="V929" s="33" t="s">
-        <v>1311</v>
+        <v>1309</v>
       </c>
     </row>
     <row r="930" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -39320,7 +39309,7 @@
       <c r="T930" s="7"/>
       <c r="U930" s="7"/>
       <c r="V930" s="33" t="s">
-        <v>1241</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="931" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -39687,7 +39676,7 @@
       <c r="T941" s="7"/>
       <c r="U941" s="7"/>
       <c r="V941" s="34" t="s">
-        <v>1493</v>
+        <v>1491</v>
       </c>
     </row>
     <row r="942" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -39753,7 +39742,7 @@
       <c r="T943" s="7"/>
       <c r="U943" s="7"/>
       <c r="V943" s="33" t="s">
-        <v>1312</v>
+        <v>1310</v>
       </c>
     </row>
     <row r="944" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -39788,7 +39777,7 @@
       <c r="T944" s="7"/>
       <c r="U944" s="7"/>
       <c r="V944" s="33" t="s">
-        <v>1313</v>
+        <v>1311</v>
       </c>
     </row>
     <row r="945" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -39856,7 +39845,7 @@
       <c r="T946" s="7"/>
       <c r="U946" s="7"/>
       <c r="V946" s="33" t="s">
-        <v>1314</v>
+        <v>1312</v>
       </c>
     </row>
     <row r="947" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -39992,7 +39981,7 @@
       <c r="T950" s="7"/>
       <c r="U950" s="7"/>
       <c r="V950" s="33" t="s">
-        <v>1315</v>
+        <v>1313</v>
       </c>
     </row>
     <row r="951" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -40359,7 +40348,7 @@
       <c r="T961" s="7"/>
       <c r="U961" s="7"/>
       <c r="V961" s="33" t="s">
-        <v>1316</v>
+        <v>1314</v>
       </c>
     </row>
     <row r="962" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -40559,7 +40548,7 @@
       <c r="T967" s="7"/>
       <c r="U967" s="7"/>
       <c r="V967" s="33" t="s">
-        <v>1317</v>
+        <v>1315</v>
       </c>
     </row>
     <row r="968" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -40664,7 +40653,7 @@
       <c r="T970" s="7"/>
       <c r="U970" s="7"/>
       <c r="V970" s="34" t="s">
-        <v>1318</v>
+        <v>1316</v>
       </c>
     </row>
     <row r="971" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -40701,7 +40690,7 @@
         <v>80</v>
       </c>
       <c r="T971" s="61" t="s">
-        <v>1489</v>
+        <v>1487</v>
       </c>
       <c r="U971" s="7"/>
       <c r="V971" s="33" t="s">
@@ -40818,7 +40807,7 @@
       <c r="T974" s="7"/>
       <c r="U974" s="7"/>
       <c r="V974" s="33" t="s">
-        <v>1319</v>
+        <v>1317</v>
       </c>
     </row>
     <row r="975" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -40886,7 +40875,7 @@
       <c r="T976" s="7"/>
       <c r="U976" s="7"/>
       <c r="V976" s="33" t="s">
-        <v>1320</v>
+        <v>1318</v>
       </c>
     </row>
     <row r="977" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -40954,7 +40943,7 @@
       <c r="T978" s="7"/>
       <c r="U978" s="7"/>
       <c r="V978" s="33" t="s">
-        <v>1321</v>
+        <v>1319</v>
       </c>
     </row>
     <row r="979" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -41128,7 +41117,7 @@
       <c r="T982" s="7"/>
       <c r="U982" s="7"/>
       <c r="V982" s="33" t="s">
-        <v>1322</v>
+        <v>1320</v>
       </c>
     </row>
     <row r="983" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -41207,7 +41196,7 @@
       <c r="T984" s="7"/>
       <c r="U984" s="7"/>
       <c r="V984" s="34" t="s">
-        <v>1323</v>
+        <v>1321</v>
       </c>
     </row>
     <row r="985" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -41390,7 +41379,7 @@
       <c r="T989" s="7"/>
       <c r="U989" s="7"/>
       <c r="V989" s="33" t="s">
-        <v>1324</v>
+        <v>1322</v>
       </c>
     </row>
     <row r="990" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -41522,7 +41511,7 @@
       <c r="T993" s="7"/>
       <c r="U993" s="7"/>
       <c r="V993" s="33" t="s">
-        <v>1325</v>
+        <v>1323</v>
       </c>
     </row>
     <row r="994" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -41623,7 +41612,7 @@
       <c r="T996" s="7"/>
       <c r="U996" s="7"/>
       <c r="V996" s="33" t="s">
-        <v>1326</v>
+        <v>1324</v>
       </c>
     </row>
     <row r="997" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -41931,7 +41920,7 @@
       <c r="T1005" s="7"/>
       <c r="U1005" s="7"/>
       <c r="V1005" s="33" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
     </row>
     <row r="1006" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -42340,7 +42329,7 @@
       <c r="T1017" s="7"/>
       <c r="U1017" s="7"/>
       <c r="V1017" s="33" t="s">
-        <v>1328</v>
+        <v>1326</v>
       </c>
     </row>
     <row r="1018" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -42616,7 +42605,7 @@
       <c r="T1025" s="7"/>
       <c r="U1025" s="7"/>
       <c r="V1025" s="33" t="s">
-        <v>1329</v>
+        <v>1327</v>
       </c>
     </row>
     <row r="1026" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -42649,7 +42638,7 @@
       <c r="T1026" s="7"/>
       <c r="U1026" s="7"/>
       <c r="V1026" s="33" t="s">
-        <v>1330</v>
+        <v>1328</v>
       </c>
     </row>
     <row r="1027" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -42717,7 +42706,7 @@
       <c r="T1028" s="7"/>
       <c r="U1028" s="7"/>
       <c r="V1028" s="33" t="s">
-        <v>1331</v>
+        <v>1329</v>
       </c>
     </row>
     <row r="1029" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -42785,7 +42774,7 @@
       <c r="T1030" s="7"/>
       <c r="U1030" s="7"/>
       <c r="V1030" s="33" t="s">
-        <v>1332</v>
+        <v>1330</v>
       </c>
     </row>
     <row r="1031" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -42853,7 +42842,7 @@
       <c r="T1032" s="7"/>
       <c r="U1032" s="7"/>
       <c r="V1032" s="33" t="s">
-        <v>1333</v>
+        <v>1331</v>
       </c>
     </row>
     <row r="1033" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -42921,7 +42910,7 @@
       <c r="T1034" s="7"/>
       <c r="U1034" s="7"/>
       <c r="V1034" s="33" t="s">
-        <v>1334</v>
+        <v>1332</v>
       </c>
     </row>
     <row r="1035" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -42989,7 +42978,7 @@
       <c r="T1036" s="7"/>
       <c r="U1036" s="7"/>
       <c r="V1036" s="33" t="s">
-        <v>1335</v>
+        <v>1333</v>
       </c>
     </row>
     <row r="1037" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -43325,7 +43314,7 @@
       <c r="T1046" s="7"/>
       <c r="U1046" s="7"/>
       <c r="V1046" s="34" t="s">
-        <v>1336</v>
+        <v>1334</v>
       </c>
     </row>
     <row r="1047" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -43492,7 +43481,7 @@
       <c r="T1051" s="7"/>
       <c r="U1051" s="7"/>
       <c r="V1051" s="33" t="s">
-        <v>1337</v>
+        <v>1335</v>
       </c>
     </row>
     <row r="1052" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -43659,7 +43648,7 @@
       <c r="T1056" s="7"/>
       <c r="U1056" s="7"/>
       <c r="V1056" s="33" t="s">
-        <v>1338</v>
+        <v>1336</v>
       </c>
     </row>
     <row r="1057" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -43694,7 +43683,7 @@
       <c r="T1057" s="7"/>
       <c r="U1057" s="7"/>
       <c r="V1057" s="33" t="s">
-        <v>1339</v>
+        <v>1337</v>
       </c>
     </row>
     <row r="1058" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -43927,7 +43916,7 @@
       <c r="T1064" s="7"/>
       <c r="U1064" s="7"/>
       <c r="V1064" s="33" t="s">
-        <v>1340</v>
+        <v>1338</v>
       </c>
     </row>
     <row r="1065" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -43962,7 +43951,7 @@
       <c r="T1065" s="7"/>
       <c r="U1065" s="7"/>
       <c r="V1065" s="33" t="s">
-        <v>1341</v>
+        <v>1339</v>
       </c>
     </row>
     <row r="1066" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -43997,7 +43986,7 @@
       <c r="T1066" s="7"/>
       <c r="U1066" s="7"/>
       <c r="V1066" s="33" t="s">
-        <v>1342</v>
+        <v>1340</v>
       </c>
     </row>
     <row r="1067" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -44034,7 +44023,7 @@
       <c r="T1067" s="7"/>
       <c r="U1067" s="7"/>
       <c r="V1067" s="33" t="s">
-        <v>1343</v>
+        <v>1341</v>
       </c>
     </row>
     <row r="1068" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -44144,7 +44133,7 @@
       <c r="T1070" s="7"/>
       <c r="U1070" s="7"/>
       <c r="V1070" s="33" t="s">
-        <v>1344</v>
+        <v>1342</v>
       </c>
     </row>
     <row r="1071" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -44552,7 +44541,7 @@
       <c r="T1082" s="7"/>
       <c r="U1082" s="7"/>
       <c r="V1082" s="33" t="s">
-        <v>1345</v>
+        <v>1343</v>
       </c>
     </row>
     <row r="1083" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -44930,7 +44919,7 @@
       <c r="T1093" s="7"/>
       <c r="U1093" s="7"/>
       <c r="V1093" s="33" t="s">
-        <v>1346</v>
+        <v>1344</v>
       </c>
     </row>
     <row r="1094" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -45112,7 +45101,7 @@
       <c r="T1098" s="7"/>
       <c r="U1098" s="7"/>
       <c r="V1098" s="33" t="s">
-        <v>1347</v>
+        <v>1345</v>
       </c>
     </row>
     <row r="1099" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -45354,7 +45343,7 @@
       <c r="T1105" s="7"/>
       <c r="U1105" s="7"/>
       <c r="V1105" s="33" t="s">
-        <v>1348</v>
+        <v>1346</v>
       </c>
     </row>
     <row r="1106" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -45724,7 +45713,7 @@
       <c r="T1116" s="7"/>
       <c r="U1116" s="7"/>
       <c r="V1116" s="33" t="s">
-        <v>1346</v>
+        <v>1344</v>
       </c>
     </row>
     <row r="1117" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -46002,7 +45991,7 @@
       <c r="T1124" s="7"/>
       <c r="U1124" s="7"/>
       <c r="V1124" s="33" t="s">
-        <v>1349</v>
+        <v>1347</v>
       </c>
     </row>
     <row r="1125" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -46281,7 +46270,7 @@
       <c r="T1132" s="7"/>
       <c r="U1132" s="7"/>
       <c r="V1132" s="33" t="s">
-        <v>1350</v>
+        <v>1348</v>
       </c>
     </row>
     <row r="1133" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -46653,7 +46642,7 @@
       <c r="T1143" s="7"/>
       <c r="U1143" s="7"/>
       <c r="V1143" s="33" t="s">
-        <v>1346</v>
+        <v>1344</v>
       </c>
     </row>
     <row r="1144" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -46719,7 +46708,7 @@
       <c r="T1145" s="7"/>
       <c r="U1145" s="7"/>
       <c r="V1145" s="33" t="s">
-        <v>1351</v>
+        <v>1349</v>
       </c>
     </row>
     <row r="1146" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -46820,7 +46809,7 @@
       <c r="T1148" s="7"/>
       <c r="U1148" s="7"/>
       <c r="V1148" s="33" t="s">
-        <v>1352</v>
+        <v>1350</v>
       </c>
     </row>
     <row r="1149" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -46892,7 +46881,7 @@
       <c r="T1150" s="7"/>
       <c r="U1150" s="7"/>
       <c r="V1150" s="33" t="s">
-        <v>1353</v>
+        <v>1351</v>
       </c>
     </row>
     <row r="1151" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -46997,7 +46986,7 @@
       <c r="S1153" s="7"/>
       <c r="T1153" s="7"/>
       <c r="V1153" s="33" t="s">
-        <v>1354</v>
+        <v>1352</v>
       </c>
     </row>
     <row r="1154" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -47173,7 +47162,7 @@
       <c r="T1158" s="7"/>
       <c r="U1158" s="7"/>
       <c r="V1158" s="33" t="s">
-        <v>1355</v>
+        <v>1353</v>
       </c>
     </row>
     <row r="1159" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -47543,7 +47532,7 @@
       <c r="T1169" s="7"/>
       <c r="U1169" s="7"/>
       <c r="V1169" s="33" t="s">
-        <v>1346</v>
+        <v>1344</v>
       </c>
     </row>
     <row r="1170" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -47646,7 +47635,7 @@
       <c r="T1172" s="7"/>
       <c r="U1172" s="7"/>
       <c r="V1172" s="33" t="s">
-        <v>1356</v>
+        <v>1354</v>
       </c>
     </row>
     <row r="1173" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -47747,7 +47736,7 @@
       <c r="T1175" s="7"/>
       <c r="U1175" s="7"/>
       <c r="V1175" s="33" t="s">
-        <v>1357</v>
+        <v>1355</v>
       </c>
     </row>
     <row r="1176" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -47848,7 +47837,7 @@
       <c r="T1178" s="7"/>
       <c r="U1178" s="7"/>
       <c r="V1178" s="33" t="s">
-        <v>1358</v>
+        <v>1356</v>
       </c>
     </row>
     <row r="1179" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -48048,7 +48037,7 @@
       <c r="T1184" s="7"/>
       <c r="U1184" s="7"/>
       <c r="V1184" s="33" t="s">
-        <v>1359</v>
+        <v>1357</v>
       </c>
     </row>
     <row r="1185" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -48415,7 +48404,7 @@
       <c r="T1195" s="7"/>
       <c r="U1195" s="7"/>
       <c r="V1195" s="33" t="s">
-        <v>1346</v>
+        <v>1344</v>
       </c>
     </row>
     <row r="1196" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -48516,7 +48505,7 @@
       <c r="T1198" s="7"/>
       <c r="U1198" s="7"/>
       <c r="V1198" s="33" t="s">
-        <v>1360</v>
+        <v>1358</v>
       </c>
     </row>
     <row r="1199" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -48551,7 +48540,7 @@
       <c r="T1199" s="7"/>
       <c r="U1199" s="7"/>
       <c r="V1199" s="33" t="s">
-        <v>1361</v>
+        <v>1359</v>
       </c>
     </row>
     <row r="1200" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -48652,7 +48641,7 @@
       <c r="T1202" s="7"/>
       <c r="U1202" s="7"/>
       <c r="V1202" s="33" t="s">
-        <v>1344</v>
+        <v>1342</v>
       </c>
     </row>
     <row r="1203" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -48720,7 +48709,7 @@
       <c r="T1204" s="7"/>
       <c r="U1204" s="7"/>
       <c r="V1204" s="33" t="s">
-        <v>1362</v>
+        <v>1360</v>
       </c>
     </row>
     <row r="1205" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -49071,7 +49060,7 @@
       <c r="T1214" s="7"/>
       <c r="U1214" s="7"/>
       <c r="V1214" s="33" t="s">
-        <v>1363</v>
+        <v>1361</v>
       </c>
     </row>
     <row r="1215" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -49438,7 +49427,7 @@
       <c r="T1225" s="7"/>
       <c r="U1225" s="7"/>
       <c r="V1225" s="33" t="s">
-        <v>1346</v>
+        <v>1344</v>
       </c>
     </row>
     <row r="1226" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -49572,7 +49561,7 @@
       <c r="T1229" s="7"/>
       <c r="U1229" s="7"/>
       <c r="V1229" s="33" t="s">
-        <v>1364</v>
+        <v>1362</v>
       </c>
     </row>
     <row r="1230" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -49778,7 +49767,7 @@
       <c r="T1235" s="7"/>
       <c r="U1235" s="7"/>
       <c r="V1235" s="33" t="s">
-        <v>1365</v>
+        <v>1363</v>
       </c>
     </row>
     <row r="1236" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -50079,7 +50068,7 @@
       <c r="T1244" s="7"/>
       <c r="U1244" s="7"/>
       <c r="V1244" s="33" t="s">
-        <v>1366</v>
+        <v>1364</v>
       </c>
     </row>
     <row r="1245" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -50394,7 +50383,7 @@
       <c r="T1253" s="7"/>
       <c r="U1253" s="7"/>
       <c r="V1253" s="33" t="s">
-        <v>1367</v>
+        <v>1365</v>
       </c>
     </row>
     <row r="1254" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -50501,7 +50490,7 @@
       <c r="T1256" s="7"/>
       <c r="U1256" s="7"/>
       <c r="V1256" s="33" t="s">
-        <v>1368</v>
+        <v>1366</v>
       </c>
     </row>
     <row r="1257" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -50706,7 +50695,7 @@
       <c r="T1262" s="7"/>
       <c r="U1262" s="7"/>
       <c r="V1262" s="33" t="s">
-        <v>1362</v>
+        <v>1360</v>
       </c>
     </row>
     <row r="1263" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -50940,7 +50929,7 @@
       <c r="T1269" s="7"/>
       <c r="U1269" s="7"/>
       <c r="V1269" s="33" t="s">
-        <v>1369</v>
+        <v>1367</v>
       </c>
     </row>
     <row r="1270" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -50977,7 +50966,7 @@
       <c r="T1270" s="7"/>
       <c r="U1270" s="7"/>
       <c r="V1270" s="33" t="s">
-        <v>1370</v>
+        <v>1368</v>
       </c>
     </row>
     <row r="1271" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -51405,7 +51394,7 @@
       <c r="T1282" s="7"/>
       <c r="U1282" s="7"/>
       <c r="V1282" s="33" t="s">
-        <v>1371</v>
+        <v>1369</v>
       </c>
     </row>
     <row r="1283" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -51506,7 +51495,7 @@
       <c r="T1285" s="7"/>
       <c r="U1285" s="7"/>
       <c r="V1285" s="33" t="s">
-        <v>1372</v>
+        <v>1370</v>
       </c>
     </row>
     <row r="1286" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -51697,7 +51686,7 @@
       <c r="T1290" s="7"/>
       <c r="U1290" s="7"/>
       <c r="V1290" s="33" t="s">
-        <v>1373</v>
+        <v>1371</v>
       </c>
     </row>
     <row r="1291" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -51949,7 +51938,7 @@
       <c r="T1297" s="7"/>
       <c r="U1297" s="7"/>
       <c r="V1297" s="33" t="s">
-        <v>1374</v>
+        <v>1372</v>
       </c>
     </row>
     <row r="1298" spans="6:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -52250,7 +52239,7 @@
       <c r="T1306" s="7"/>
       <c r="U1306" s="7"/>
       <c r="V1306" s="33" t="s">
-        <v>1375</v>
+        <v>1373</v>
       </c>
     </row>
     <row r="1307" spans="6:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -52588,7 +52577,7 @@
       <c r="T1316" s="7"/>
       <c r="U1316" s="7"/>
       <c r="V1316" s="33" t="s">
-        <v>1376</v>
+        <v>1374</v>
       </c>
     </row>
     <row r="1317" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -52623,7 +52612,7 @@
       <c r="T1317" s="7"/>
       <c r="U1317" s="7"/>
       <c r="V1317" s="33" t="s">
-        <v>1377</v>
+        <v>1375</v>
       </c>
     </row>
     <row r="1318" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -52658,7 +52647,7 @@
       <c r="T1318" s="7"/>
       <c r="U1318" s="7"/>
       <c r="V1318" s="33" t="s">
-        <v>1378</v>
+        <v>1376</v>
       </c>
     </row>
     <row r="1319" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -52933,7 +52922,7 @@
       <c r="T1326" s="7"/>
       <c r="U1326" s="7"/>
       <c r="V1326" s="33" t="s">
-        <v>1379</v>
+        <v>1377</v>
       </c>
     </row>
     <row r="1327" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -53075,7 +53064,7 @@
       <c r="T1330" s="7"/>
       <c r="U1330" s="7"/>
       <c r="V1330" s="33" t="s">
-        <v>1380</v>
+        <v>1378</v>
       </c>
     </row>
     <row r="1331" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -53181,7 +53170,7 @@
       <c r="S1333" s="7"/>
       <c r="T1333" s="7"/>
       <c r="V1333" s="33" t="s">
-        <v>1381</v>
+        <v>1379</v>
       </c>
     </row>
     <row r="1334" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -53249,7 +53238,7 @@
       <c r="S1335" s="7"/>
       <c r="T1335" s="7"/>
       <c r="V1335" s="34" t="s">
-        <v>1382</v>
+        <v>1380</v>
       </c>
     </row>
     <row r="1336" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -53350,7 +53339,7 @@
       <c r="T1338" s="7"/>
       <c r="U1338" s="7"/>
       <c r="V1338" s="33" t="s">
-        <v>1383</v>
+        <v>1381</v>
       </c>
     </row>
     <row r="1339" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -53519,7 +53508,7 @@
       <c r="T1343" s="7"/>
       <c r="U1343" s="7"/>
       <c r="V1343" s="44" t="s">
-        <v>1384</v>
+        <v>1382</v>
       </c>
     </row>
     <row r="1344" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -53546,7 +53535,7 @@
         <v>1</v>
       </c>
       <c r="N1344" s="34" t="s">
-        <v>1494</v>
+        <v>1492</v>
       </c>
       <c r="O1344" s="6"/>
       <c r="P1344" s="7"/>
@@ -53741,7 +53730,7 @@
       <c r="T1349" s="7"/>
       <c r="U1349" s="7"/>
       <c r="V1349" s="33" t="s">
-        <v>1385</v>
+        <v>1383</v>
       </c>
     </row>
     <row r="1350" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -53779,7 +53768,7 @@
       <c r="T1350" s="7"/>
       <c r="U1350" s="7"/>
       <c r="V1350" s="33" t="s">
-        <v>1386</v>
+        <v>1384</v>
       </c>
     </row>
     <row r="1351" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -53855,7 +53844,7 @@
         <v>81</v>
       </c>
       <c r="V1352" s="33" t="s">
-        <v>1387</v>
+        <v>1385</v>
       </c>
     </row>
     <row r="1353" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -53965,7 +53954,7 @@
       <c r="T1355" s="7"/>
       <c r="U1355" s="7"/>
       <c r="V1355" s="33" t="s">
-        <v>1388</v>
+        <v>1386</v>
       </c>
     </row>
     <row r="1356" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -54003,7 +53992,7 @@
       <c r="T1356" s="7"/>
       <c r="U1356" s="7"/>
       <c r="V1356" s="33" t="s">
-        <v>1389</v>
+        <v>1387</v>
       </c>
     </row>
     <row r="1357" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -54114,7 +54103,7 @@
       <c r="T1359" s="7"/>
       <c r="U1359" s="7"/>
       <c r="V1359" s="33" t="s">
-        <v>1390</v>
+        <v>1388</v>
       </c>
     </row>
     <row r="1360" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -54416,7 +54405,7 @@
       <c r="T1367" s="7"/>
       <c r="U1367" s="7"/>
       <c r="V1367" s="33" t="s">
-        <v>1391</v>
+        <v>1389</v>
       </c>
     </row>
     <row r="1368" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -54532,7 +54521,7 @@
       <c r="T1370" s="7"/>
       <c r="U1370" s="7"/>
       <c r="V1370" s="33" t="s">
-        <v>1392</v>
+        <v>1390</v>
       </c>
     </row>
     <row r="1371" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -54647,7 +54636,7 @@
       <c r="T1373" s="7"/>
       <c r="U1373" s="7"/>
       <c r="V1373" s="33" t="s">
-        <v>1393</v>
+        <v>1391</v>
       </c>
     </row>
     <row r="1374" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -54832,7 +54821,7 @@
       <c r="T1378" s="7"/>
       <c r="U1378" s="7"/>
       <c r="V1378" s="33" t="s">
-        <v>1394</v>
+        <v>1392</v>
       </c>
     </row>
     <row r="1379" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -54870,7 +54859,7 @@
       <c r="T1379" s="7"/>
       <c r="U1379" s="7"/>
       <c r="V1379" s="33" t="s">
-        <v>1395</v>
+        <v>1393</v>
       </c>
     </row>
     <row r="1380" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -55207,7 +55196,7 @@
       <c r="T1388" s="7"/>
       <c r="U1388" s="7"/>
       <c r="V1388" s="33" t="s">
-        <v>1396</v>
+        <v>1394</v>
       </c>
     </row>
     <row r="1389" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -55574,7 +55563,7 @@
       <c r="T1398" s="7"/>
       <c r="U1398" s="7"/>
       <c r="V1398" s="33" t="s">
-        <v>1397</v>
+        <v>1395</v>
       </c>
     </row>
     <row r="1399" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -55961,7 +55950,7 @@
       <c r="T1408" s="7"/>
       <c r="U1408" s="7"/>
       <c r="V1408" s="33" t="s">
-        <v>1398</v>
+        <v>1396</v>
       </c>
     </row>
     <row r="1409" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -56194,7 +56183,7 @@
       <c r="T1414" s="7"/>
       <c r="U1414" s="7"/>
       <c r="V1414" s="33" t="s">
-        <v>1399</v>
+        <v>1397</v>
       </c>
     </row>
     <row r="1415" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -56342,7 +56331,7 @@
       <c r="T1418" s="7"/>
       <c r="U1418" s="7"/>
       <c r="V1418" s="33" t="s">
-        <v>1362</v>
+        <v>1360</v>
       </c>
     </row>
     <row r="1419" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -56380,7 +56369,7 @@
       <c r="T1419" s="7"/>
       <c r="U1419" s="7"/>
       <c r="V1419" s="33" t="s">
-        <v>1400</v>
+        <v>1398</v>
       </c>
     </row>
     <row r="1420" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -56600,7 +56589,7 @@
       <c r="T1425" s="7"/>
       <c r="U1425" s="7"/>
       <c r="V1425" s="33" t="s">
-        <v>1401</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="1426" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -56710,7 +56699,7 @@
       <c r="T1428" s="7"/>
       <c r="U1428" s="7"/>
       <c r="V1428" s="33" t="s">
-        <v>1402</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="1429" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -56902,7 +56891,7 @@
         <v>85</v>
       </c>
       <c r="V1433" s="33" t="s">
-        <v>1403</v>
+        <v>1401</v>
       </c>
     </row>
     <row r="1434" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -57021,7 +57010,7 @@
       <c r="T1436" s="7"/>
       <c r="U1436" s="7"/>
       <c r="V1436" s="33" t="s">
-        <v>1404</v>
+        <v>1402</v>
       </c>
     </row>
     <row r="1437" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -57502,7 +57491,7 @@
       <c r="T1448" s="7"/>
       <c r="U1448" s="7"/>
       <c r="V1448" s="33" t="s">
-        <v>1405</v>
+        <v>1403</v>
       </c>
     </row>
     <row r="1449" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -57832,7 +57821,7 @@
       <c r="T1457" s="7"/>
       <c r="U1457" s="7"/>
       <c r="V1457" s="33" t="s">
-        <v>1406</v>
+        <v>1404</v>
       </c>
     </row>
     <row r="1458" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -57985,7 +57974,7 @@
       <c r="T1461" s="7"/>
       <c r="U1461" s="7"/>
       <c r="V1461" s="33" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
     </row>
     <row r="1462" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -58314,7 +58303,7 @@
       <c r="T1470" s="7"/>
       <c r="U1470" s="7"/>
       <c r="V1470" s="33" t="s">
-        <v>1407</v>
+        <v>1405</v>
       </c>
     </row>
     <row r="1471" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -58352,7 +58341,7 @@
       <c r="T1471" s="7"/>
       <c r="U1471" s="7"/>
       <c r="V1471" s="33" t="s">
-        <v>1408</v>
+        <v>1406</v>
       </c>
     </row>
     <row r="1472" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -58390,7 +58379,7 @@
       <c r="T1472" s="7"/>
       <c r="U1472" s="7"/>
       <c r="V1472" s="33" t="s">
-        <v>1409</v>
+        <v>1407</v>
       </c>
     </row>
     <row r="1473" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -58501,7 +58490,7 @@
       <c r="T1475" s="7"/>
       <c r="U1475" s="7"/>
       <c r="V1475" s="33" t="s">
-        <v>1410</v>
+        <v>1408</v>
       </c>
     </row>
     <row r="1476" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -59090,7 +59079,7 @@
       <c r="T1491" s="7"/>
       <c r="U1491" s="7"/>
       <c r="V1491" s="34" t="s">
-        <v>1487</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="1492" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -59348,7 +59337,7 @@
         <v>8</v>
       </c>
       <c r="N1499" s="34" t="s">
-        <v>1495</v>
+        <v>1493</v>
       </c>
       <c r="O1499" s="6" t="s">
         <v>72</v>
@@ -59360,7 +59349,7 @@
       <c r="T1499" s="7"/>
       <c r="U1499" s="7"/>
       <c r="V1499" s="33" t="s">
-        <v>1411</v>
+        <v>1409</v>
       </c>
     </row>
     <row r="1500" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -59398,7 +59387,7 @@
       <c r="T1500" s="7"/>
       <c r="U1500" s="7"/>
       <c r="V1500" s="33" t="s">
-        <v>1412</v>
+        <v>1410</v>
       </c>
     </row>
     <row r="1501" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -59509,7 +59498,7 @@
       <c r="T1503" s="7"/>
       <c r="U1503" s="7"/>
       <c r="V1503" s="33" t="s">
-        <v>1413</v>
+        <v>1411</v>
       </c>
     </row>
     <row r="1504" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -59624,7 +59613,7 @@
       <c r="T1506" s="7"/>
       <c r="U1506" s="7"/>
       <c r="V1506" s="33" t="s">
-        <v>1414</v>
+        <v>1412</v>
       </c>
     </row>
     <row r="1507" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -59662,7 +59651,7 @@
       <c r="T1507" s="7"/>
       <c r="U1507" s="7"/>
       <c r="V1507" s="34" t="s">
-        <v>1415</v>
+        <v>1413</v>
       </c>
     </row>
     <row r="1508" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -59700,7 +59689,7 @@
       <c r="T1508" s="7"/>
       <c r="U1508" s="7"/>
       <c r="V1508" s="34" t="s">
-        <v>1496</v>
+        <v>1494</v>
       </c>
     </row>
     <row r="1509" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -59973,7 +59962,7 @@
       </c>
       <c r="U1516" s="7"/>
       <c r="V1516" s="33" t="s">
-        <v>1274</v>
+        <v>1272</v>
       </c>
     </row>
     <row r="1517" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -60044,7 +60033,7 @@
         <v>81</v>
       </c>
       <c r="V1518" s="33" t="s">
-        <v>1416</v>
+        <v>1414</v>
       </c>
     </row>
     <row r="1519" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -60145,7 +60134,7 @@
       <c r="T1521" s="7"/>
       <c r="U1521" s="7"/>
       <c r="V1521" s="33" t="s">
-        <v>1417</v>
+        <v>1415</v>
       </c>
     </row>
     <row r="1522" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -60380,7 +60369,7 @@
       <c r="T1528" s="7"/>
       <c r="U1528" s="7"/>
       <c r="V1528" s="33" t="s">
-        <v>1418</v>
+        <v>1416</v>
       </c>
     </row>
     <row r="1529" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -60415,7 +60404,7 @@
       <c r="T1529" s="7"/>
       <c r="U1529" s="7"/>
       <c r="V1529" s="33" t="s">
-        <v>1419</v>
+        <v>1417</v>
       </c>
     </row>
     <row r="1530" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -60650,7 +60639,7 @@
       <c r="T1536" s="7"/>
       <c r="U1536" s="7"/>
       <c r="V1536" s="34" t="s">
-        <v>1497</v>
+        <v>1495</v>
       </c>
     </row>
     <row r="1537" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -60760,7 +60749,7 @@
       <c r="T1539" s="7"/>
       <c r="U1539" s="7"/>
       <c r="V1539" s="33" t="s">
-        <v>1420</v>
+        <v>1418</v>
       </c>
     </row>
     <row r="1540" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -60831,7 +60820,7 @@
       <c r="T1541" s="7"/>
       <c r="U1541" s="7"/>
       <c r="V1541" s="33" t="s">
-        <v>1421</v>
+        <v>1419</v>
       </c>
     </row>
     <row r="1542" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -60865,7 +60854,7 @@
       <c r="T1542" s="7"/>
       <c r="U1542" s="7"/>
       <c r="V1542" s="33" t="s">
-        <v>1422</v>
+        <v>1420</v>
       </c>
     </row>
     <row r="1543" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -60933,7 +60922,7 @@
       <c r="T1544" s="7"/>
       <c r="U1544" s="7"/>
       <c r="V1544" s="33" t="s">
-        <v>1423</v>
+        <v>1421</v>
       </c>
     </row>
     <row r="1545" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -61284,7 +61273,7 @@
       <c r="T1554" s="7"/>
       <c r="U1554" s="7"/>
       <c r="V1554" s="33" t="s">
-        <v>1424</v>
+        <v>1422</v>
       </c>
     </row>
     <row r="1555" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -61329,7 +61318,7 @@
       </c>
       <c r="U1555" s="7"/>
       <c r="V1555" s="33" t="s">
-        <v>1425</v>
+        <v>1423</v>
       </c>
     </row>
     <row r="1556" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -61636,7 +61625,7 @@
       <c r="T1564" s="7"/>
       <c r="U1564" s="7"/>
       <c r="V1564" s="33" t="s">
-        <v>1407</v>
+        <v>1405</v>
       </c>
     </row>
     <row r="1565" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -61676,7 +61665,7 @@
       <c r="T1565" s="7"/>
       <c r="U1565" s="7"/>
       <c r="V1565" s="33" t="s">
-        <v>1426</v>
+        <v>1424</v>
       </c>
     </row>
     <row r="1566" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -61711,7 +61700,7 @@
       <c r="T1566" s="7"/>
       <c r="U1566" s="7"/>
       <c r="V1566" s="33" t="s">
-        <v>1427</v>
+        <v>1425</v>
       </c>
     </row>
     <row r="1567" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -61746,7 +61735,7 @@
       <c r="T1567" s="7"/>
       <c r="U1567" s="7"/>
       <c r="V1567" s="33" t="s">
-        <v>1428</v>
+        <v>1426</v>
       </c>
     </row>
     <row r="1568" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -61815,7 +61804,7 @@
       <c r="T1569" s="7"/>
       <c r="U1569" s="7"/>
       <c r="V1569" s="33" t="s">
-        <v>1429</v>
+        <v>1427</v>
       </c>
     </row>
     <row r="1570" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -61850,7 +61839,7 @@
       <c r="T1570" s="7"/>
       <c r="U1570" s="7"/>
       <c r="V1570" s="33" t="s">
-        <v>1430</v>
+        <v>1428</v>
       </c>
     </row>
     <row r="1571" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -61885,7 +61874,7 @@
       <c r="T1571" s="7"/>
       <c r="U1571" s="7"/>
       <c r="V1571" s="33" t="s">
-        <v>1431</v>
+        <v>1429</v>
       </c>
     </row>
     <row r="1572" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -61953,7 +61942,7 @@
       <c r="T1573" s="7"/>
       <c r="U1573" s="7"/>
       <c r="V1573" s="33" t="s">
-        <v>1430</v>
+        <v>1428</v>
       </c>
     </row>
     <row r="1574" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -62059,7 +62048,7 @@
       <c r="T1576" s="7"/>
       <c r="U1576" s="7"/>
       <c r="V1576" s="33" t="s">
-        <v>1393</v>
+        <v>1391</v>
       </c>
     </row>
     <row r="1577" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -62237,7 +62226,7 @@
         <v>72</v>
       </c>
       <c r="V1581" s="33" t="s">
-        <v>1432</v>
+        <v>1430</v>
       </c>
     </row>
     <row r="1582" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -62449,7 +62438,7 @@
         <v>72</v>
       </c>
       <c r="V1588" s="33" t="s">
-        <v>1433</v>
+        <v>1431</v>
       </c>
     </row>
     <row r="1589" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -62581,7 +62570,7 @@
         <v>72</v>
       </c>
       <c r="V1593" s="33" t="s">
-        <v>1434</v>
+        <v>1432</v>
       </c>
     </row>
     <row r="1594" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -63026,7 +63015,7 @@
         <v>72</v>
       </c>
       <c r="V1610" s="33" t="s">
-        <v>1435</v>
+        <v>1433</v>
       </c>
     </row>
     <row r="1611" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -63055,7 +63044,7 @@
         <v>72</v>
       </c>
       <c r="V1611" s="33" t="s">
-        <v>1436</v>
+        <v>1434</v>
       </c>
     </row>
     <row r="1612" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -63162,7 +63151,7 @@
         <v>72</v>
       </c>
       <c r="V1615" s="33" t="s">
-        <v>1437</v>
+        <v>1435</v>
       </c>
     </row>
     <row r="1616" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -63217,7 +63206,7 @@
         <v>72</v>
       </c>
       <c r="V1617" s="33" t="s">
-        <v>1438</v>
+        <v>1436</v>
       </c>
     </row>
     <row r="1618" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -63298,7 +63287,7 @@
         <v>72</v>
       </c>
       <c r="V1620" s="33" t="s">
-        <v>1439</v>
+        <v>1437</v>
       </c>
     </row>
     <row r="1621" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -63469,7 +63458,7 @@
         <v>72</v>
       </c>
       <c r="V1626" s="33" t="s">
-        <v>1440</v>
+        <v>1438</v>
       </c>
     </row>
     <row r="1627" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -63814,7 +63803,7 @@
         <v>73</v>
       </c>
       <c r="V1638" s="33" t="s">
-        <v>1441</v>
+        <v>1439</v>
       </c>
     </row>
     <row r="1639" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -64064,7 +64053,7 @@
         <v>73</v>
       </c>
       <c r="V1647" s="33" t="s">
-        <v>1442</v>
+        <v>1440</v>
       </c>
     </row>
     <row r="1648" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -64318,7 +64307,7 @@
         <v>73</v>
       </c>
       <c r="V1655" s="33" t="s">
-        <v>1443</v>
+        <v>1441</v>
       </c>
     </row>
     <row r="1656" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -64350,7 +64339,7 @@
         <v>72</v>
       </c>
       <c r="V1656" s="33" t="s">
-        <v>1444</v>
+        <v>1442</v>
       </c>
     </row>
     <row r="1657" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -64472,7 +64461,7 @@
         <v>72</v>
       </c>
       <c r="V1660" s="33" t="s">
-        <v>1445</v>
+        <v>1443</v>
       </c>
     </row>
     <row r="1661" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -64539,7 +64528,7 @@
         <v>81</v>
       </c>
       <c r="V1662" s="33" t="s">
-        <v>1446</v>
+        <v>1444</v>
       </c>
     </row>
     <row r="1663" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -64571,7 +64560,7 @@
         <v>73</v>
       </c>
       <c r="V1663" s="33" t="s">
-        <v>1447</v>
+        <v>1445</v>
       </c>
     </row>
     <row r="1664" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -64661,7 +64650,7 @@
         <v>72</v>
       </c>
       <c r="V1666" s="33" t="s">
-        <v>1448</v>
+        <v>1446</v>
       </c>
     </row>
     <row r="1667" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -64696,7 +64685,7 @@
         <v>72</v>
       </c>
       <c r="V1667" s="33" t="s">
-        <v>1449</v>
+        <v>1447</v>
       </c>
     </row>
     <row r="1668" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -64864,7 +64853,7 @@
       </c>
       <c r="U1672" s="7"/>
       <c r="V1672" s="33" t="s">
-        <v>1450</v>
+        <v>1448</v>
       </c>
     </row>
     <row r="1673" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -64987,7 +64976,7 @@
         <v>72</v>
       </c>
       <c r="V1676" s="33" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
     </row>
     <row r="1677" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -65019,7 +65008,7 @@
         <v>72</v>
       </c>
       <c r="V1677" s="33" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
     </row>
     <row r="1678" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -65109,7 +65098,7 @@
         <v>73</v>
       </c>
       <c r="V1680" s="33" t="s">
-        <v>1453</v>
+        <v>1451</v>
       </c>
     </row>
     <row r="1681" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -65144,7 +65133,7 @@
         <v>74</v>
       </c>
       <c r="V1681" s="33" t="s">
-        <v>1454</v>
+        <v>1452</v>
       </c>
     </row>
     <row r="1682" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -65311,7 +65300,7 @@
         <v>73</v>
       </c>
       <c r="V1686" s="33" t="s">
-        <v>1455</v>
+        <v>1453</v>
       </c>
     </row>
     <row r="1687" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -65480,7 +65469,7 @@
         <v>73</v>
       </c>
       <c r="V1691" s="33" t="s">
-        <v>1456</v>
+        <v>1454</v>
       </c>
     </row>
     <row r="1692" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -65512,7 +65501,7 @@
         <v>72</v>
       </c>
       <c r="V1692" s="33" t="s">
-        <v>1457</v>
+        <v>1455</v>
       </c>
     </row>
     <row r="1693" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -65631,7 +65620,7 @@
         <v>72</v>
       </c>
       <c r="V1696" s="33" t="s">
-        <v>1458</v>
+        <v>1456</v>
       </c>
     </row>
     <row r="1697" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -65663,7 +65652,7 @@
         <v>72</v>
       </c>
       <c r="V1697" s="33" t="s">
-        <v>1459</v>
+        <v>1457</v>
       </c>
     </row>
     <row r="1698" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -65694,7 +65683,7 @@
         <v>73</v>
       </c>
       <c r="V1698" s="34" t="s">
-        <v>1488</v>
+        <v>1486</v>
       </c>
     </row>
     <row r="1699" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -65793,7 +65782,7 @@
         <v>72</v>
       </c>
       <c r="V1701" s="33" t="s">
-        <v>1460</v>
+        <v>1458</v>
       </c>
     </row>
     <row r="1702" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -65915,7 +65904,7 @@
         <v>72</v>
       </c>
       <c r="V1705" s="33" t="s">
-        <v>1461</v>
+        <v>1459</v>
       </c>
     </row>
     <row r="1706" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -65978,7 +65967,7 @@
       </c>
       <c r="U1707" s="7"/>
       <c r="V1707" s="33" t="s">
-        <v>1462</v>
+        <v>1460</v>
       </c>
     </row>
     <row r="1708" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -66099,7 +66088,7 @@
         <v>72</v>
       </c>
       <c r="V1711" s="33" t="s">
-        <v>1444</v>
+        <v>1442</v>
       </c>
     </row>
     <row r="1712" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -66163,7 +66152,7 @@
         <v>73</v>
       </c>
       <c r="V1713" s="33" t="s">
-        <v>1463</v>
+        <v>1461</v>
       </c>
     </row>
     <row r="1714" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -66195,7 +66184,7 @@
         <v>72</v>
       </c>
       <c r="V1714" s="33" t="s">
-        <v>1464</v>
+        <v>1462</v>
       </c>
     </row>
     <row r="1715" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -66233,7 +66222,7 @@
         <v>85</v>
       </c>
       <c r="V1715" s="33" t="s">
-        <v>1465</v>
+        <v>1463</v>
       </c>
     </row>
     <row r="1716" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -66446,7 +66435,7 @@
         <v>73</v>
       </c>
       <c r="V1721" s="33" t="s">
-        <v>1441</v>
+        <v>1439</v>
       </c>
     </row>
     <row r="1722" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -66726,7 +66715,7 @@
         <v>73</v>
       </c>
       <c r="V1730" s="33" t="s">
-        <v>1442</v>
+        <v>1440</v>
       </c>
     </row>
     <row r="1731" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -66787,7 +66776,7 @@
         <v>72</v>
       </c>
       <c r="V1732" s="33" t="s">
-        <v>1466</v>
+        <v>1464</v>
       </c>
     </row>
     <row r="1733" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -66925,7 +66914,7 @@
         <v>73</v>
       </c>
       <c r="V1736" s="33" t="s">
-        <v>1467</v>
+        <v>1465</v>
       </c>
     </row>
     <row r="1737" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -67015,7 +67004,7 @@
         <v>72</v>
       </c>
       <c r="V1739" s="33" t="s">
-        <v>1468</v>
+        <v>1466</v>
       </c>
     </row>
     <row r="1740" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -67050,7 +67039,7 @@
         <v>73</v>
       </c>
       <c r="V1740" s="33" t="s">
-        <v>1469</v>
+        <v>1467</v>
       </c>
     </row>
     <row r="1741" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -67143,7 +67132,7 @@
         <v>72</v>
       </c>
       <c r="V1743" s="33" t="s">
-        <v>1470</v>
+        <v>1468</v>
       </c>
     </row>
     <row r="1744" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -67328,7 +67317,7 @@
         <v>73</v>
       </c>
       <c r="V1749" s="33" t="s">
-        <v>1471</v>
+        <v>1469</v>
       </c>
     </row>
     <row r="1750" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -67418,7 +67407,7 @@
         <v>72</v>
       </c>
       <c r="V1752" s="33" t="s">
-        <v>1472</v>
+        <v>1470</v>
       </c>
     </row>
     <row r="1753" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -67575,7 +67564,7 @@
         <v>73</v>
       </c>
       <c r="V1757" s="33" t="s">
-        <v>1473</v>
+        <v>1471</v>
       </c>
     </row>
     <row r="1758" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -67674,7 +67663,7 @@
         <v>72</v>
       </c>
       <c r="V1760" s="33" t="s">
-        <v>1474</v>
+        <v>1472</v>
       </c>
     </row>
     <row r="1761" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -67767,7 +67756,7 @@
         <v>73</v>
       </c>
       <c r="V1763" s="34" t="s">
-        <v>1475</v>
+        <v>1473</v>
       </c>
     </row>
     <row r="1764" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -67889,7 +67878,7 @@
         <v>73</v>
       </c>
       <c r="V1767" s="33" t="s">
-        <v>1476</v>
+        <v>1474</v>
       </c>
     </row>
     <row r="1768" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -68218,7 +68207,7 @@
         <v>73</v>
       </c>
       <c r="V1777" s="33" t="s">
-        <v>1477</v>
+        <v>1475</v>
       </c>
     </row>
     <row r="1778" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -68456,7 +68445,7 @@
         <v>73</v>
       </c>
       <c r="V1785" s="33" t="s">
-        <v>1478</v>
+        <v>1476</v>
       </c>
     </row>
     <row r="1786" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -68637,7 +68626,7 @@
         <v>72</v>
       </c>
       <c r="V1791" s="34" t="s">
-        <v>1479</v>
+        <v>1477</v>
       </c>
     </row>
     <row r="1792" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -68669,7 +68658,7 @@
         <v>73</v>
       </c>
       <c r="V1792" s="33" t="s">
-        <v>1480</v>
+        <v>1478</v>
       </c>
     </row>
     <row r="1793" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -68701,7 +68690,7 @@
         <v>72</v>
       </c>
       <c r="V1793" s="33" t="s">
-        <v>1481</v>
+        <v>1479</v>
       </c>
     </row>
     <row r="1794" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -68736,7 +68725,7 @@
         <v>73</v>
       </c>
       <c r="V1794" s="33" t="s">
-        <v>1482</v>
+        <v>1480</v>
       </c>
     </row>
     <row r="1795" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -68977,7 +68966,7 @@
         <v>73</v>
       </c>
       <c r="V1802" s="33" t="s">
-        <v>1483</v>
+        <v>1481</v>
       </c>
     </row>
     <row r="1803" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -69070,7 +69059,7 @@
         <v>73</v>
       </c>
       <c r="V1805" s="33" t="s">
-        <v>1484</v>
+        <v>1482</v>
       </c>
     </row>
     <row r="1806" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -69274,7 +69263,7 @@
         <v>73</v>
       </c>
       <c r="V1811" s="33" t="s">
-        <v>1485</v>
+        <v>1483</v>
       </c>
     </row>
     <row r="1812" spans="3:22" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
nmv 11 02 2023
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Padam Input Templates/TS 1.4 Padam Input Template.xlsx
+++ b/TS Jatai Working/Padam Input Templates/TS 1.4 Padam Input Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALL IMP DATA\GitHub\texts\TS Jatai Working\Padam Input Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0051A71C-7171-45EA-9748-CC61ED98A925}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{217466FC-8EDC-4B59-85A3-239D86CAF043}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6750" uniqueCount="1497">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6754" uniqueCount="1497">
   <si>
     <t>Passage</t>
   </si>
@@ -3852,9 +3852,6 @@
     <t>vaqriqvoqvittaqreti# varivoqvit - taqrAq</t>
   </si>
   <si>
-    <t>asaqdiyasa#t</t>
-  </si>
-  <si>
     <t>soqmaqpIqtha iti# soma - pIqthaH</t>
   </si>
   <si>
@@ -3952,9 +3949,6 @@
   </si>
   <si>
     <t>Sipreq itiq Sipre$</t>
-  </si>
-  <si>
-    <t>aqveqpaqyaq iti# avepayaH</t>
   </si>
   <si>
     <t>caqmU iti# caqmU</t>
@@ -4658,6 +4652,12 @@
   </si>
   <si>
     <t>BUqditi# BUt</t>
+  </si>
+  <si>
+    <t>asaqdityasa#t</t>
+  </si>
+  <si>
+    <t>aqveqpaqyaq itya#vepayaH</t>
   </si>
 </sst>
 </file>
@@ -5342,10 +5342,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V1812"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A689" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="V695" sqref="V695"/>
+      <selection pane="bottomLeft" activeCell="N926" sqref="N926"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -31322,7 +31322,7 @@
       <c r="T697" s="7"/>
       <c r="U697" s="7"/>
       <c r="V697" s="34" t="s">
-        <v>1496</v>
+        <v>1494</v>
       </c>
     </row>
     <row r="698" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -33413,7 +33413,7 @@
         <v>52</v>
       </c>
       <c r="N758" s="34" t="s">
-        <v>1488</v>
+        <v>1486</v>
       </c>
       <c r="O758" s="6" t="s">
         <v>72</v>
@@ -33631,8 +33631,8 @@
       <c r="S764" s="7"/>
       <c r="T764" s="7"/>
       <c r="U764" s="7"/>
-      <c r="V764" s="33" t="s">
-        <v>1274</v>
+      <c r="V764" s="34" t="s">
+        <v>1495</v>
       </c>
     </row>
     <row r="765" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -33800,7 +33800,7 @@
       <c r="T769" s="7"/>
       <c r="U769" s="7"/>
       <c r="V769" s="33" t="s">
-        <v>1275</v>
+        <v>1274</v>
       </c>
     </row>
     <row r="770" spans="6:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -34266,7 +34266,7 @@
       <c r="T783" s="7"/>
       <c r="U783" s="7"/>
       <c r="V783" s="33" t="s">
-        <v>1276</v>
+        <v>1275</v>
       </c>
     </row>
     <row r="784" spans="6:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -34513,7 +34513,7 @@
       <c r="T790" s="7"/>
       <c r="U790" s="7"/>
       <c r="V790" s="33" t="s">
-        <v>1277</v>
+        <v>1276</v>
       </c>
     </row>
     <row r="791" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -34584,7 +34584,7 @@
       <c r="T792" s="7"/>
       <c r="U792" s="7"/>
       <c r="V792" s="33" t="s">
-        <v>1278</v>
+        <v>1277</v>
       </c>
     </row>
     <row r="793" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -34619,7 +34619,7 @@
       <c r="T793" s="7"/>
       <c r="U793" s="7"/>
       <c r="V793" s="33" t="s">
-        <v>1279</v>
+        <v>1278</v>
       </c>
     </row>
     <row r="794" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -34898,7 +34898,7 @@
       <c r="T801" s="7"/>
       <c r="U801" s="7"/>
       <c r="V801" s="33" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
     </row>
     <row r="802" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -34935,7 +34935,7 @@
       <c r="T802" s="7"/>
       <c r="U802" s="7"/>
       <c r="V802" s="33" t="s">
-        <v>1281</v>
+        <v>1280</v>
       </c>
     </row>
     <row r="803" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -35105,7 +35105,7 @@
       <c r="T807" s="7"/>
       <c r="U807" s="7"/>
       <c r="V807" s="34" t="s">
-        <v>1489</v>
+        <v>1487</v>
       </c>
     </row>
     <row r="808" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -35212,7 +35212,7 @@
       </c>
       <c r="U810" s="7"/>
       <c r="V810" s="33" t="s">
-        <v>1282</v>
+        <v>1281</v>
       </c>
     </row>
     <row r="811" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -35482,7 +35482,7 @@
       <c r="T818" s="7"/>
       <c r="U818" s="7"/>
       <c r="V818" s="33" t="s">
-        <v>1283</v>
+        <v>1282</v>
       </c>
     </row>
     <row r="819" spans="6:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -35704,7 +35704,7 @@
         <v>81</v>
       </c>
       <c r="V824" s="33" t="s">
-        <v>1284</v>
+        <v>1283</v>
       </c>
     </row>
     <row r="825" spans="6:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -35739,7 +35739,7 @@
       <c r="T825" s="7"/>
       <c r="U825" s="7"/>
       <c r="V825" s="33" t="s">
-        <v>1285</v>
+        <v>1284</v>
       </c>
     </row>
     <row r="826" spans="6:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -35908,7 +35908,7 @@
       <c r="T830" s="7"/>
       <c r="U830" s="7"/>
       <c r="V830" s="34" t="s">
-        <v>1484</v>
+        <v>1482</v>
       </c>
     </row>
     <row r="831" spans="6:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -35941,7 +35941,7 @@
       <c r="T831" s="7"/>
       <c r="U831" s="7"/>
       <c r="V831" s="33" t="s">
-        <v>1286</v>
+        <v>1285</v>
       </c>
     </row>
     <row r="832" spans="6:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -36077,7 +36077,7 @@
       <c r="T835" s="7"/>
       <c r="U835" s="7"/>
       <c r="V835" s="33" t="s">
-        <v>1287</v>
+        <v>1286</v>
       </c>
     </row>
     <row r="836" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -36211,7 +36211,7 @@
       <c r="T839" s="7"/>
       <c r="U839" s="7"/>
       <c r="V839" s="33" t="s">
-        <v>1288</v>
+        <v>1287</v>
       </c>
     </row>
     <row r="840" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -36380,7 +36380,7 @@
       <c r="T844" s="7"/>
       <c r="U844" s="7"/>
       <c r="V844" s="34" t="s">
-        <v>1489</v>
+        <v>1487</v>
       </c>
     </row>
     <row r="845" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -36413,7 +36413,7 @@
       <c r="T845" s="7"/>
       <c r="U845" s="7"/>
       <c r="V845" s="33" t="s">
-        <v>1289</v>
+        <v>1288</v>
       </c>
     </row>
     <row r="846" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -36484,7 +36484,7 @@
       <c r="T847" s="7"/>
       <c r="U847" s="7"/>
       <c r="V847" s="33" t="s">
-        <v>1290</v>
+        <v>1289</v>
       </c>
     </row>
     <row r="848" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -36819,7 +36819,7 @@
       <c r="T857" s="7"/>
       <c r="U857" s="7"/>
       <c r="V857" s="33" t="s">
-        <v>1291</v>
+        <v>1290</v>
       </c>
     </row>
     <row r="858" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -36887,7 +36887,7 @@
       <c r="T859" s="7"/>
       <c r="U859" s="7"/>
       <c r="V859" s="33" t="s">
-        <v>1292</v>
+        <v>1291</v>
       </c>
     </row>
     <row r="860" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -36922,7 +36922,7 @@
       <c r="T860" s="7"/>
       <c r="U860" s="7"/>
       <c r="V860" s="33" t="s">
-        <v>1293</v>
+        <v>1292</v>
       </c>
     </row>
     <row r="861" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -36957,7 +36957,7 @@
       <c r="T861" s="7"/>
       <c r="U861" s="7"/>
       <c r="V861" s="33" t="s">
-        <v>1294</v>
+        <v>1293</v>
       </c>
     </row>
     <row r="862" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -37086,7 +37086,7 @@
         <v>9</v>
       </c>
       <c r="N865" s="34" t="s">
-        <v>1490</v>
+        <v>1488</v>
       </c>
       <c r="O865" s="6" t="s">
         <v>72</v>
@@ -37098,7 +37098,7 @@
       <c r="T865" s="7"/>
       <c r="U865" s="7"/>
       <c r="V865" s="33" t="s">
-        <v>1295</v>
+        <v>1294</v>
       </c>
     </row>
     <row r="866" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -37133,7 +37133,7 @@
       <c r="T866" s="7"/>
       <c r="U866" s="7"/>
       <c r="V866" s="33" t="s">
-        <v>1296</v>
+        <v>1295</v>
       </c>
     </row>
     <row r="867" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -37399,7 +37399,7 @@
       <c r="T874" s="7"/>
       <c r="U874" s="7"/>
       <c r="V874" s="33" t="s">
-        <v>1297</v>
+        <v>1296</v>
       </c>
     </row>
     <row r="875" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -37765,7 +37765,7 @@
       <c r="T885" s="7"/>
       <c r="U885" s="7"/>
       <c r="V885" s="33" t="s">
-        <v>1298</v>
+        <v>1297</v>
       </c>
     </row>
     <row r="886" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -37800,7 +37800,7 @@
       <c r="T886" s="7"/>
       <c r="U886" s="7"/>
       <c r="V886" s="33" t="s">
-        <v>1299</v>
+        <v>1298</v>
       </c>
     </row>
     <row r="887" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -37835,7 +37835,7 @@
       <c r="T887" s="7"/>
       <c r="U887" s="7"/>
       <c r="V887" s="33" t="s">
-        <v>1300</v>
+        <v>1299</v>
       </c>
     </row>
     <row r="888" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -37870,7 +37870,7 @@
       <c r="T888" s="7"/>
       <c r="U888" s="7"/>
       <c r="V888" s="33" t="s">
-        <v>1301</v>
+        <v>1300</v>
       </c>
     </row>
     <row r="889" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -38103,7 +38103,7 @@
       <c r="T895" s="7"/>
       <c r="U895" s="7"/>
       <c r="V895" s="33" t="s">
-        <v>1302</v>
+        <v>1301</v>
       </c>
     </row>
     <row r="896" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -38475,7 +38475,7 @@
       <c r="T906" s="7"/>
       <c r="U906" s="7"/>
       <c r="V906" s="33" t="s">
-        <v>1303</v>
+        <v>1302</v>
       </c>
     </row>
     <row r="907" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -38579,7 +38579,7 @@
       <c r="T909" s="7"/>
       <c r="U909" s="7"/>
       <c r="V909" s="33" t="s">
-        <v>1304</v>
+        <v>1303</v>
       </c>
     </row>
     <row r="910" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -38951,7 +38951,7 @@
       <c r="T920" s="7"/>
       <c r="U920" s="7"/>
       <c r="V920" s="33" t="s">
-        <v>1305</v>
+        <v>1304</v>
       </c>
     </row>
     <row r="921" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -38987,7 +38987,7 @@
       <c r="T921" s="7"/>
       <c r="U921" s="7"/>
       <c r="V921" s="33" t="s">
-        <v>1306</v>
+        <v>1305</v>
       </c>
     </row>
     <row r="922" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -39133,7 +39133,7 @@
       <c r="T925" s="7"/>
       <c r="U925" s="7"/>
       <c r="V925" s="33" t="s">
-        <v>1307</v>
+        <v>1306</v>
       </c>
     </row>
     <row r="926" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -39158,7 +39158,7 @@
         <f t="shared" si="30"/>
         <v>6</v>
       </c>
-      <c r="N926" s="33" t="s">
+      <c r="N926" s="34" t="s">
         <v>660</v>
       </c>
       <c r="O926" s="6"/>
@@ -39172,8 +39172,8 @@
       <c r="U926" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="V926" s="33" t="s">
-        <v>1308</v>
+      <c r="V926" s="34" t="s">
+        <v>1496</v>
       </c>
     </row>
     <row r="927" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -39274,7 +39274,7 @@
       <c r="T929" s="7"/>
       <c r="U929" s="7"/>
       <c r="V929" s="33" t="s">
-        <v>1309</v>
+        <v>1307</v>
       </c>
     </row>
     <row r="930" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -39676,7 +39676,7 @@
       <c r="T941" s="7"/>
       <c r="U941" s="7"/>
       <c r="V941" s="34" t="s">
-        <v>1491</v>
+        <v>1489</v>
       </c>
     </row>
     <row r="942" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -39742,7 +39742,7 @@
       <c r="T943" s="7"/>
       <c r="U943" s="7"/>
       <c r="V943" s="33" t="s">
-        <v>1310</v>
+        <v>1308</v>
       </c>
     </row>
     <row r="944" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -39777,7 +39777,7 @@
       <c r="T944" s="7"/>
       <c r="U944" s="7"/>
       <c r="V944" s="33" t="s">
-        <v>1311</v>
+        <v>1309</v>
       </c>
     </row>
     <row r="945" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -39845,7 +39845,7 @@
       <c r="T946" s="7"/>
       <c r="U946" s="7"/>
       <c r="V946" s="33" t="s">
-        <v>1312</v>
+        <v>1310</v>
       </c>
     </row>
     <row r="947" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -39981,7 +39981,7 @@
       <c r="T950" s="7"/>
       <c r="U950" s="7"/>
       <c r="V950" s="33" t="s">
-        <v>1313</v>
+        <v>1311</v>
       </c>
     </row>
     <row r="951" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -40348,7 +40348,7 @@
       <c r="T961" s="7"/>
       <c r="U961" s="7"/>
       <c r="V961" s="33" t="s">
-        <v>1314</v>
+        <v>1312</v>
       </c>
     </row>
     <row r="962" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -40548,7 +40548,7 @@
       <c r="T967" s="7"/>
       <c r="U967" s="7"/>
       <c r="V967" s="33" t="s">
-        <v>1315</v>
+        <v>1313</v>
       </c>
     </row>
     <row r="968" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -40653,7 +40653,7 @@
       <c r="T970" s="7"/>
       <c r="U970" s="7"/>
       <c r="V970" s="34" t="s">
-        <v>1316</v>
+        <v>1314</v>
       </c>
     </row>
     <row r="971" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -40690,7 +40690,7 @@
         <v>80</v>
       </c>
       <c r="T971" s="61" t="s">
-        <v>1487</v>
+        <v>1485</v>
       </c>
       <c r="U971" s="7"/>
       <c r="V971" s="33" t="s">
@@ -40807,7 +40807,7 @@
       <c r="T974" s="7"/>
       <c r="U974" s="7"/>
       <c r="V974" s="33" t="s">
-        <v>1317</v>
+        <v>1315</v>
       </c>
     </row>
     <row r="975" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -40875,7 +40875,7 @@
       <c r="T976" s="7"/>
       <c r="U976" s="7"/>
       <c r="V976" s="33" t="s">
-        <v>1318</v>
+        <v>1316</v>
       </c>
     </row>
     <row r="977" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -40943,7 +40943,7 @@
       <c r="T978" s="7"/>
       <c r="U978" s="7"/>
       <c r="V978" s="33" t="s">
-        <v>1319</v>
+        <v>1317</v>
       </c>
     </row>
     <row r="979" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -41117,7 +41117,7 @@
       <c r="T982" s="7"/>
       <c r="U982" s="7"/>
       <c r="V982" s="33" t="s">
-        <v>1320</v>
+        <v>1318</v>
       </c>
     </row>
     <row r="983" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -41196,7 +41196,7 @@
       <c r="T984" s="7"/>
       <c r="U984" s="7"/>
       <c r="V984" s="34" t="s">
-        <v>1321</v>
+        <v>1319</v>
       </c>
     </row>
     <row r="985" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -41379,7 +41379,7 @@
       <c r="T989" s="7"/>
       <c r="U989" s="7"/>
       <c r="V989" s="33" t="s">
-        <v>1322</v>
+        <v>1320</v>
       </c>
     </row>
     <row r="990" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -41511,7 +41511,7 @@
       <c r="T993" s="7"/>
       <c r="U993" s="7"/>
       <c r="V993" s="33" t="s">
-        <v>1323</v>
+        <v>1321</v>
       </c>
     </row>
     <row r="994" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -41612,7 +41612,7 @@
       <c r="T996" s="7"/>
       <c r="U996" s="7"/>
       <c r="V996" s="33" t="s">
-        <v>1324</v>
+        <v>1322</v>
       </c>
     </row>
     <row r="997" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -41920,7 +41920,7 @@
       <c r="T1005" s="7"/>
       <c r="U1005" s="7"/>
       <c r="V1005" s="33" t="s">
-        <v>1325</v>
+        <v>1323</v>
       </c>
     </row>
     <row r="1006" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -42329,7 +42329,7 @@
       <c r="T1017" s="7"/>
       <c r="U1017" s="7"/>
       <c r="V1017" s="33" t="s">
-        <v>1326</v>
+        <v>1324</v>
       </c>
     </row>
     <row r="1018" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -42605,7 +42605,7 @@
       <c r="T1025" s="7"/>
       <c r="U1025" s="7"/>
       <c r="V1025" s="33" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
     </row>
     <row r="1026" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -42638,7 +42638,7 @@
       <c r="T1026" s="7"/>
       <c r="U1026" s="7"/>
       <c r="V1026" s="33" t="s">
-        <v>1328</v>
+        <v>1326</v>
       </c>
     </row>
     <row r="1027" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -42706,7 +42706,7 @@
       <c r="T1028" s="7"/>
       <c r="U1028" s="7"/>
       <c r="V1028" s="33" t="s">
-        <v>1329</v>
+        <v>1327</v>
       </c>
     </row>
     <row r="1029" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -42774,7 +42774,7 @@
       <c r="T1030" s="7"/>
       <c r="U1030" s="7"/>
       <c r="V1030" s="33" t="s">
-        <v>1330</v>
+        <v>1328</v>
       </c>
     </row>
     <row r="1031" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -42842,7 +42842,7 @@
       <c r="T1032" s="7"/>
       <c r="U1032" s="7"/>
       <c r="V1032" s="33" t="s">
-        <v>1331</v>
+        <v>1329</v>
       </c>
     </row>
     <row r="1033" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -42910,7 +42910,7 @@
       <c r="T1034" s="7"/>
       <c r="U1034" s="7"/>
       <c r="V1034" s="33" t="s">
-        <v>1332</v>
+        <v>1330</v>
       </c>
     </row>
     <row r="1035" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -42978,7 +42978,7 @@
       <c r="T1036" s="7"/>
       <c r="U1036" s="7"/>
       <c r="V1036" s="33" t="s">
-        <v>1333</v>
+        <v>1331</v>
       </c>
     </row>
     <row r="1037" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -43314,7 +43314,7 @@
       <c r="T1046" s="7"/>
       <c r="U1046" s="7"/>
       <c r="V1046" s="34" t="s">
-        <v>1334</v>
+        <v>1332</v>
       </c>
     </row>
     <row r="1047" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -43481,7 +43481,7 @@
       <c r="T1051" s="7"/>
       <c r="U1051" s="7"/>
       <c r="V1051" s="33" t="s">
-        <v>1335</v>
+        <v>1333</v>
       </c>
     </row>
     <row r="1052" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -43648,7 +43648,7 @@
       <c r="T1056" s="7"/>
       <c r="U1056" s="7"/>
       <c r="V1056" s="33" t="s">
-        <v>1336</v>
+        <v>1334</v>
       </c>
     </row>
     <row r="1057" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -43683,7 +43683,7 @@
       <c r="T1057" s="7"/>
       <c r="U1057" s="7"/>
       <c r="V1057" s="33" t="s">
-        <v>1337</v>
+        <v>1335</v>
       </c>
     </row>
     <row r="1058" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -43916,7 +43916,7 @@
       <c r="T1064" s="7"/>
       <c r="U1064" s="7"/>
       <c r="V1064" s="33" t="s">
-        <v>1338</v>
+        <v>1336</v>
       </c>
     </row>
     <row r="1065" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -43951,7 +43951,7 @@
       <c r="T1065" s="7"/>
       <c r="U1065" s="7"/>
       <c r="V1065" s="33" t="s">
-        <v>1339</v>
+        <v>1337</v>
       </c>
     </row>
     <row r="1066" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -43986,7 +43986,7 @@
       <c r="T1066" s="7"/>
       <c r="U1066" s="7"/>
       <c r="V1066" s="33" t="s">
-        <v>1340</v>
+        <v>1338</v>
       </c>
     </row>
     <row r="1067" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -44023,7 +44023,7 @@
       <c r="T1067" s="7"/>
       <c r="U1067" s="7"/>
       <c r="V1067" s="33" t="s">
-        <v>1341</v>
+        <v>1339</v>
       </c>
     </row>
     <row r="1068" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -44133,7 +44133,7 @@
       <c r="T1070" s="7"/>
       <c r="U1070" s="7"/>
       <c r="V1070" s="33" t="s">
-        <v>1342</v>
+        <v>1340</v>
       </c>
     </row>
     <row r="1071" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -44541,7 +44541,7 @@
       <c r="T1082" s="7"/>
       <c r="U1082" s="7"/>
       <c r="V1082" s="33" t="s">
-        <v>1343</v>
+        <v>1341</v>
       </c>
     </row>
     <row r="1083" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -44919,7 +44919,7 @@
       <c r="T1093" s="7"/>
       <c r="U1093" s="7"/>
       <c r="V1093" s="33" t="s">
-        <v>1344</v>
+        <v>1342</v>
       </c>
     </row>
     <row r="1094" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -45101,7 +45101,7 @@
       <c r="T1098" s="7"/>
       <c r="U1098" s="7"/>
       <c r="V1098" s="33" t="s">
-        <v>1345</v>
+        <v>1343</v>
       </c>
     </row>
     <row r="1099" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -45343,7 +45343,7 @@
       <c r="T1105" s="7"/>
       <c r="U1105" s="7"/>
       <c r="V1105" s="33" t="s">
-        <v>1346</v>
+        <v>1344</v>
       </c>
     </row>
     <row r="1106" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -45713,7 +45713,7 @@
       <c r="T1116" s="7"/>
       <c r="U1116" s="7"/>
       <c r="V1116" s="33" t="s">
-        <v>1344</v>
+        <v>1342</v>
       </c>
     </row>
     <row r="1117" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -45991,7 +45991,7 @@
       <c r="T1124" s="7"/>
       <c r="U1124" s="7"/>
       <c r="V1124" s="33" t="s">
-        <v>1347</v>
+        <v>1345</v>
       </c>
     </row>
     <row r="1125" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -46270,7 +46270,7 @@
       <c r="T1132" s="7"/>
       <c r="U1132" s="7"/>
       <c r="V1132" s="33" t="s">
-        <v>1348</v>
+        <v>1346</v>
       </c>
     </row>
     <row r="1133" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -46642,7 +46642,7 @@
       <c r="T1143" s="7"/>
       <c r="U1143" s="7"/>
       <c r="V1143" s="33" t="s">
-        <v>1344</v>
+        <v>1342</v>
       </c>
     </row>
     <row r="1144" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -46708,7 +46708,7 @@
       <c r="T1145" s="7"/>
       <c r="U1145" s="7"/>
       <c r="V1145" s="33" t="s">
-        <v>1349</v>
+        <v>1347</v>
       </c>
     </row>
     <row r="1146" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -46809,7 +46809,7 @@
       <c r="T1148" s="7"/>
       <c r="U1148" s="7"/>
       <c r="V1148" s="33" t="s">
-        <v>1350</v>
+        <v>1348</v>
       </c>
     </row>
     <row r="1149" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -46881,7 +46881,7 @@
       <c r="T1150" s="7"/>
       <c r="U1150" s="7"/>
       <c r="V1150" s="33" t="s">
-        <v>1351</v>
+        <v>1349</v>
       </c>
     </row>
     <row r="1151" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -46986,7 +46986,7 @@
       <c r="S1153" s="7"/>
       <c r="T1153" s="7"/>
       <c r="V1153" s="33" t="s">
-        <v>1352</v>
+        <v>1350</v>
       </c>
     </row>
     <row r="1154" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -47162,7 +47162,7 @@
       <c r="T1158" s="7"/>
       <c r="U1158" s="7"/>
       <c r="V1158" s="33" t="s">
-        <v>1353</v>
+        <v>1351</v>
       </c>
     </row>
     <row r="1159" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -47532,7 +47532,7 @@
       <c r="T1169" s="7"/>
       <c r="U1169" s="7"/>
       <c r="V1169" s="33" t="s">
-        <v>1344</v>
+        <v>1342</v>
       </c>
     </row>
     <row r="1170" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -47635,7 +47635,7 @@
       <c r="T1172" s="7"/>
       <c r="U1172" s="7"/>
       <c r="V1172" s="33" t="s">
-        <v>1354</v>
+        <v>1352</v>
       </c>
     </row>
     <row r="1173" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -47736,7 +47736,7 @@
       <c r="T1175" s="7"/>
       <c r="U1175" s="7"/>
       <c r="V1175" s="33" t="s">
-        <v>1355</v>
+        <v>1353</v>
       </c>
     </row>
     <row r="1176" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -47837,7 +47837,7 @@
       <c r="T1178" s="7"/>
       <c r="U1178" s="7"/>
       <c r="V1178" s="33" t="s">
-        <v>1356</v>
+        <v>1354</v>
       </c>
     </row>
     <row r="1179" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -48037,7 +48037,7 @@
       <c r="T1184" s="7"/>
       <c r="U1184" s="7"/>
       <c r="V1184" s="33" t="s">
-        <v>1357</v>
+        <v>1355</v>
       </c>
     </row>
     <row r="1185" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -48404,7 +48404,7 @@
       <c r="T1195" s="7"/>
       <c r="U1195" s="7"/>
       <c r="V1195" s="33" t="s">
-        <v>1344</v>
+        <v>1342</v>
       </c>
     </row>
     <row r="1196" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -48505,7 +48505,7 @@
       <c r="T1198" s="7"/>
       <c r="U1198" s="7"/>
       <c r="V1198" s="33" t="s">
-        <v>1358</v>
+        <v>1356</v>
       </c>
     </row>
     <row r="1199" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -48540,7 +48540,7 @@
       <c r="T1199" s="7"/>
       <c r="U1199" s="7"/>
       <c r="V1199" s="33" t="s">
-        <v>1359</v>
+        <v>1357</v>
       </c>
     </row>
     <row r="1200" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -48641,7 +48641,7 @@
       <c r="T1202" s="7"/>
       <c r="U1202" s="7"/>
       <c r="V1202" s="33" t="s">
-        <v>1342</v>
+        <v>1340</v>
       </c>
     </row>
     <row r="1203" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -48709,7 +48709,7 @@
       <c r="T1204" s="7"/>
       <c r="U1204" s="7"/>
       <c r="V1204" s="33" t="s">
-        <v>1360</v>
+        <v>1358</v>
       </c>
     </row>
     <row r="1205" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -49060,7 +49060,7 @@
       <c r="T1214" s="7"/>
       <c r="U1214" s="7"/>
       <c r="V1214" s="33" t="s">
-        <v>1361</v>
+        <v>1359</v>
       </c>
     </row>
     <row r="1215" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -49427,7 +49427,7 @@
       <c r="T1225" s="7"/>
       <c r="U1225" s="7"/>
       <c r="V1225" s="33" t="s">
-        <v>1344</v>
+        <v>1342</v>
       </c>
     </row>
     <row r="1226" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -49561,7 +49561,7 @@
       <c r="T1229" s="7"/>
       <c r="U1229" s="7"/>
       <c r="V1229" s="33" t="s">
-        <v>1362</v>
+        <v>1360</v>
       </c>
     </row>
     <row r="1230" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -49767,7 +49767,7 @@
       <c r="T1235" s="7"/>
       <c r="U1235" s="7"/>
       <c r="V1235" s="33" t="s">
-        <v>1363</v>
+        <v>1361</v>
       </c>
     </row>
     <row r="1236" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -50068,7 +50068,7 @@
       <c r="T1244" s="7"/>
       <c r="U1244" s="7"/>
       <c r="V1244" s="33" t="s">
-        <v>1364</v>
+        <v>1362</v>
       </c>
     </row>
     <row r="1245" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -50383,7 +50383,7 @@
       <c r="T1253" s="7"/>
       <c r="U1253" s="7"/>
       <c r="V1253" s="33" t="s">
-        <v>1365</v>
+        <v>1363</v>
       </c>
     </row>
     <row r="1254" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -50490,7 +50490,7 @@
       <c r="T1256" s="7"/>
       <c r="U1256" s="7"/>
       <c r="V1256" s="33" t="s">
-        <v>1366</v>
+        <v>1364</v>
       </c>
     </row>
     <row r="1257" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -50695,7 +50695,7 @@
       <c r="T1262" s="7"/>
       <c r="U1262" s="7"/>
       <c r="V1262" s="33" t="s">
-        <v>1360</v>
+        <v>1358</v>
       </c>
     </row>
     <row r="1263" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -50929,7 +50929,7 @@
       <c r="T1269" s="7"/>
       <c r="U1269" s="7"/>
       <c r="V1269" s="33" t="s">
-        <v>1367</v>
+        <v>1365</v>
       </c>
     </row>
     <row r="1270" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -50966,7 +50966,7 @@
       <c r="T1270" s="7"/>
       <c r="U1270" s="7"/>
       <c r="V1270" s="33" t="s">
-        <v>1368</v>
+        <v>1366</v>
       </c>
     </row>
     <row r="1271" spans="5:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -51394,7 +51394,7 @@
       <c r="T1282" s="7"/>
       <c r="U1282" s="7"/>
       <c r="V1282" s="33" t="s">
-        <v>1369</v>
+        <v>1367</v>
       </c>
     </row>
     <row r="1283" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -51495,7 +51495,7 @@
       <c r="T1285" s="7"/>
       <c r="U1285" s="7"/>
       <c r="V1285" s="33" t="s">
-        <v>1370</v>
+        <v>1368</v>
       </c>
     </row>
     <row r="1286" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -51686,7 +51686,7 @@
       <c r="T1290" s="7"/>
       <c r="U1290" s="7"/>
       <c r="V1290" s="33" t="s">
-        <v>1371</v>
+        <v>1369</v>
       </c>
     </row>
     <row r="1291" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -51938,7 +51938,7 @@
       <c r="T1297" s="7"/>
       <c r="U1297" s="7"/>
       <c r="V1297" s="33" t="s">
-        <v>1372</v>
+        <v>1370</v>
       </c>
     </row>
     <row r="1298" spans="6:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -52239,7 +52239,7 @@
       <c r="T1306" s="7"/>
       <c r="U1306" s="7"/>
       <c r="V1306" s="33" t="s">
-        <v>1373</v>
+        <v>1371</v>
       </c>
     </row>
     <row r="1307" spans="6:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -52577,7 +52577,7 @@
       <c r="T1316" s="7"/>
       <c r="U1316" s="7"/>
       <c r="V1316" s="33" t="s">
-        <v>1374</v>
+        <v>1372</v>
       </c>
     </row>
     <row r="1317" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -52612,7 +52612,7 @@
       <c r="T1317" s="7"/>
       <c r="U1317" s="7"/>
       <c r="V1317" s="33" t="s">
-        <v>1375</v>
+        <v>1373</v>
       </c>
     </row>
     <row r="1318" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -52647,7 +52647,7 @@
       <c r="T1318" s="7"/>
       <c r="U1318" s="7"/>
       <c r="V1318" s="33" t="s">
-        <v>1376</v>
+        <v>1374</v>
       </c>
     </row>
     <row r="1319" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -52922,7 +52922,7 @@
       <c r="T1326" s="7"/>
       <c r="U1326" s="7"/>
       <c r="V1326" s="33" t="s">
-        <v>1377</v>
+        <v>1375</v>
       </c>
     </row>
     <row r="1327" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -53064,7 +53064,7 @@
       <c r="T1330" s="7"/>
       <c r="U1330" s="7"/>
       <c r="V1330" s="33" t="s">
-        <v>1378</v>
+        <v>1376</v>
       </c>
     </row>
     <row r="1331" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -53170,7 +53170,7 @@
       <c r="S1333" s="7"/>
       <c r="T1333" s="7"/>
       <c r="V1333" s="33" t="s">
-        <v>1379</v>
+        <v>1377</v>
       </c>
     </row>
     <row r="1334" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -53238,7 +53238,7 @@
       <c r="S1335" s="7"/>
       <c r="T1335" s="7"/>
       <c r="V1335" s="34" t="s">
-        <v>1380</v>
+        <v>1378</v>
       </c>
     </row>
     <row r="1336" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -53339,7 +53339,7 @@
       <c r="T1338" s="7"/>
       <c r="U1338" s="7"/>
       <c r="V1338" s="33" t="s">
-        <v>1381</v>
+        <v>1379</v>
       </c>
     </row>
     <row r="1339" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -53508,7 +53508,7 @@
       <c r="T1343" s="7"/>
       <c r="U1343" s="7"/>
       <c r="V1343" s="44" t="s">
-        <v>1382</v>
+        <v>1380</v>
       </c>
     </row>
     <row r="1344" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -53535,7 +53535,7 @@
         <v>1</v>
       </c>
       <c r="N1344" s="34" t="s">
-        <v>1492</v>
+        <v>1490</v>
       </c>
       <c r="O1344" s="6"/>
       <c r="P1344" s="7"/>
@@ -53730,7 +53730,7 @@
       <c r="T1349" s="7"/>
       <c r="U1349" s="7"/>
       <c r="V1349" s="33" t="s">
-        <v>1383</v>
+        <v>1381</v>
       </c>
     </row>
     <row r="1350" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -53768,7 +53768,7 @@
       <c r="T1350" s="7"/>
       <c r="U1350" s="7"/>
       <c r="V1350" s="33" t="s">
-        <v>1384</v>
+        <v>1382</v>
       </c>
     </row>
     <row r="1351" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -53844,7 +53844,7 @@
         <v>81</v>
       </c>
       <c r="V1352" s="33" t="s">
-        <v>1385</v>
+        <v>1383</v>
       </c>
     </row>
     <row r="1353" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -53954,7 +53954,7 @@
       <c r="T1355" s="7"/>
       <c r="U1355" s="7"/>
       <c r="V1355" s="33" t="s">
-        <v>1386</v>
+        <v>1384</v>
       </c>
     </row>
     <row r="1356" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -53992,7 +53992,7 @@
       <c r="T1356" s="7"/>
       <c r="U1356" s="7"/>
       <c r="V1356" s="33" t="s">
-        <v>1387</v>
+        <v>1385</v>
       </c>
     </row>
     <row r="1357" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -54103,7 +54103,7 @@
       <c r="T1359" s="7"/>
       <c r="U1359" s="7"/>
       <c r="V1359" s="33" t="s">
-        <v>1388</v>
+        <v>1386</v>
       </c>
     </row>
     <row r="1360" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -54405,7 +54405,7 @@
       <c r="T1367" s="7"/>
       <c r="U1367" s="7"/>
       <c r="V1367" s="33" t="s">
-        <v>1389</v>
+        <v>1387</v>
       </c>
     </row>
     <row r="1368" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -54521,7 +54521,7 @@
       <c r="T1370" s="7"/>
       <c r="U1370" s="7"/>
       <c r="V1370" s="33" t="s">
-        <v>1390</v>
+        <v>1388</v>
       </c>
     </row>
     <row r="1371" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -54636,7 +54636,7 @@
       <c r="T1373" s="7"/>
       <c r="U1373" s="7"/>
       <c r="V1373" s="33" t="s">
-        <v>1391</v>
+        <v>1389</v>
       </c>
     </row>
     <row r="1374" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -54821,7 +54821,7 @@
       <c r="T1378" s="7"/>
       <c r="U1378" s="7"/>
       <c r="V1378" s="33" t="s">
-        <v>1392</v>
+        <v>1390</v>
       </c>
     </row>
     <row r="1379" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -54859,7 +54859,7 @@
       <c r="T1379" s="7"/>
       <c r="U1379" s="7"/>
       <c r="V1379" s="33" t="s">
-        <v>1393</v>
+        <v>1391</v>
       </c>
     </row>
     <row r="1380" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -55196,7 +55196,7 @@
       <c r="T1388" s="7"/>
       <c r="U1388" s="7"/>
       <c r="V1388" s="33" t="s">
-        <v>1394</v>
+        <v>1392</v>
       </c>
     </row>
     <row r="1389" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -55563,7 +55563,7 @@
       <c r="T1398" s="7"/>
       <c r="U1398" s="7"/>
       <c r="V1398" s="33" t="s">
-        <v>1395</v>
+        <v>1393</v>
       </c>
     </row>
     <row r="1399" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -55950,7 +55950,7 @@
       <c r="T1408" s="7"/>
       <c r="U1408" s="7"/>
       <c r="V1408" s="33" t="s">
-        <v>1396</v>
+        <v>1394</v>
       </c>
     </row>
     <row r="1409" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -56183,7 +56183,7 @@
       <c r="T1414" s="7"/>
       <c r="U1414" s="7"/>
       <c r="V1414" s="33" t="s">
-        <v>1397</v>
+        <v>1395</v>
       </c>
     </row>
     <row r="1415" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -56331,7 +56331,7 @@
       <c r="T1418" s="7"/>
       <c r="U1418" s="7"/>
       <c r="V1418" s="33" t="s">
-        <v>1360</v>
+        <v>1358</v>
       </c>
     </row>
     <row r="1419" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -56369,7 +56369,7 @@
       <c r="T1419" s="7"/>
       <c r="U1419" s="7"/>
       <c r="V1419" s="33" t="s">
-        <v>1398</v>
+        <v>1396</v>
       </c>
     </row>
     <row r="1420" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -56589,7 +56589,7 @@
       <c r="T1425" s="7"/>
       <c r="U1425" s="7"/>
       <c r="V1425" s="33" t="s">
-        <v>1399</v>
+        <v>1397</v>
       </c>
     </row>
     <row r="1426" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -56699,7 +56699,7 @@
       <c r="T1428" s="7"/>
       <c r="U1428" s="7"/>
       <c r="V1428" s="33" t="s">
-        <v>1400</v>
+        <v>1398</v>
       </c>
     </row>
     <row r="1429" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -56891,7 +56891,7 @@
         <v>85</v>
       </c>
       <c r="V1433" s="33" t="s">
-        <v>1401</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="1434" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -57010,7 +57010,7 @@
       <c r="T1436" s="7"/>
       <c r="U1436" s="7"/>
       <c r="V1436" s="33" t="s">
-        <v>1402</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="1437" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -57491,7 +57491,7 @@
       <c r="T1448" s="7"/>
       <c r="U1448" s="7"/>
       <c r="V1448" s="33" t="s">
-        <v>1403</v>
+        <v>1401</v>
       </c>
     </row>
     <row r="1449" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -57821,7 +57821,7 @@
       <c r="T1457" s="7"/>
       <c r="U1457" s="7"/>
       <c r="V1457" s="33" t="s">
-        <v>1404</v>
+        <v>1402</v>
       </c>
     </row>
     <row r="1458" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -58303,7 +58303,7 @@
       <c r="T1470" s="7"/>
       <c r="U1470" s="7"/>
       <c r="V1470" s="33" t="s">
-        <v>1405</v>
+        <v>1403</v>
       </c>
     </row>
     <row r="1471" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -58341,7 +58341,7 @@
       <c r="T1471" s="7"/>
       <c r="U1471" s="7"/>
       <c r="V1471" s="33" t="s">
-        <v>1406</v>
+        <v>1404</v>
       </c>
     </row>
     <row r="1472" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -58379,7 +58379,7 @@
       <c r="T1472" s="7"/>
       <c r="U1472" s="7"/>
       <c r="V1472" s="33" t="s">
-        <v>1407</v>
+        <v>1405</v>
       </c>
     </row>
     <row r="1473" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -58490,7 +58490,7 @@
       <c r="T1475" s="7"/>
       <c r="U1475" s="7"/>
       <c r="V1475" s="33" t="s">
-        <v>1408</v>
+        <v>1406</v>
       </c>
     </row>
     <row r="1476" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -59079,7 +59079,7 @@
       <c r="T1491" s="7"/>
       <c r="U1491" s="7"/>
       <c r="V1491" s="34" t="s">
-        <v>1485</v>
+        <v>1483</v>
       </c>
     </row>
     <row r="1492" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -59337,7 +59337,7 @@
         <v>8</v>
       </c>
       <c r="N1499" s="34" t="s">
-        <v>1493</v>
+        <v>1491</v>
       </c>
       <c r="O1499" s="6" t="s">
         <v>72</v>
@@ -59349,7 +59349,7 @@
       <c r="T1499" s="7"/>
       <c r="U1499" s="7"/>
       <c r="V1499" s="33" t="s">
-        <v>1409</v>
+        <v>1407</v>
       </c>
     </row>
     <row r="1500" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -59387,7 +59387,7 @@
       <c r="T1500" s="7"/>
       <c r="U1500" s="7"/>
       <c r="V1500" s="33" t="s">
-        <v>1410</v>
+        <v>1408</v>
       </c>
     </row>
     <row r="1501" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -59498,7 +59498,7 @@
       <c r="T1503" s="7"/>
       <c r="U1503" s="7"/>
       <c r="V1503" s="33" t="s">
-        <v>1411</v>
+        <v>1409</v>
       </c>
     </row>
     <row r="1504" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -59613,7 +59613,7 @@
       <c r="T1506" s="7"/>
       <c r="U1506" s="7"/>
       <c r="V1506" s="33" t="s">
-        <v>1412</v>
+        <v>1410</v>
       </c>
     </row>
     <row r="1507" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -59651,7 +59651,7 @@
       <c r="T1507" s="7"/>
       <c r="U1507" s="7"/>
       <c r="V1507" s="34" t="s">
-        <v>1413</v>
+        <v>1411</v>
       </c>
     </row>
     <row r="1508" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -59689,7 +59689,7 @@
       <c r="T1508" s="7"/>
       <c r="U1508" s="7"/>
       <c r="V1508" s="34" t="s">
-        <v>1494</v>
+        <v>1492</v>
       </c>
     </row>
     <row r="1509" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -60033,7 +60033,7 @@
         <v>81</v>
       </c>
       <c r="V1518" s="33" t="s">
-        <v>1414</v>
+        <v>1412</v>
       </c>
     </row>
     <row r="1519" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -60134,7 +60134,7 @@
       <c r="T1521" s="7"/>
       <c r="U1521" s="7"/>
       <c r="V1521" s="33" t="s">
-        <v>1415</v>
+        <v>1413</v>
       </c>
     </row>
     <row r="1522" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -60369,7 +60369,7 @@
       <c r="T1528" s="7"/>
       <c r="U1528" s="7"/>
       <c r="V1528" s="33" t="s">
-        <v>1416</v>
+        <v>1414</v>
       </c>
     </row>
     <row r="1529" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -60404,7 +60404,7 @@
       <c r="T1529" s="7"/>
       <c r="U1529" s="7"/>
       <c r="V1529" s="33" t="s">
-        <v>1417</v>
+        <v>1415</v>
       </c>
     </row>
     <row r="1530" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -60639,7 +60639,7 @@
       <c r="T1536" s="7"/>
       <c r="U1536" s="7"/>
       <c r="V1536" s="34" t="s">
-        <v>1495</v>
+        <v>1493</v>
       </c>
     </row>
     <row r="1537" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -60749,7 +60749,7 @@
       <c r="T1539" s="7"/>
       <c r="U1539" s="7"/>
       <c r="V1539" s="33" t="s">
-        <v>1418</v>
+        <v>1416</v>
       </c>
     </row>
     <row r="1540" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -60820,7 +60820,7 @@
       <c r="T1541" s="7"/>
       <c r="U1541" s="7"/>
       <c r="V1541" s="33" t="s">
-        <v>1419</v>
+        <v>1417</v>
       </c>
     </row>
     <row r="1542" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -60854,7 +60854,7 @@
       <c r="T1542" s="7"/>
       <c r="U1542" s="7"/>
       <c r="V1542" s="33" t="s">
-        <v>1420</v>
+        <v>1418</v>
       </c>
     </row>
     <row r="1543" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -60922,7 +60922,7 @@
       <c r="T1544" s="7"/>
       <c r="U1544" s="7"/>
       <c r="V1544" s="33" t="s">
-        <v>1421</v>
+        <v>1419</v>
       </c>
     </row>
     <row r="1545" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -61273,7 +61273,7 @@
       <c r="T1554" s="7"/>
       <c r="U1554" s="7"/>
       <c r="V1554" s="33" t="s">
-        <v>1422</v>
+        <v>1420</v>
       </c>
     </row>
     <row r="1555" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -61318,7 +61318,7 @@
       </c>
       <c r="U1555" s="7"/>
       <c r="V1555" s="33" t="s">
-        <v>1423</v>
+        <v>1421</v>
       </c>
     </row>
     <row r="1556" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -61625,7 +61625,7 @@
       <c r="T1564" s="7"/>
       <c r="U1564" s="7"/>
       <c r="V1564" s="33" t="s">
-        <v>1405</v>
+        <v>1403</v>
       </c>
     </row>
     <row r="1565" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -61665,7 +61665,7 @@
       <c r="T1565" s="7"/>
       <c r="U1565" s="7"/>
       <c r="V1565" s="33" t="s">
-        <v>1424</v>
+        <v>1422</v>
       </c>
     </row>
     <row r="1566" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -61700,7 +61700,7 @@
       <c r="T1566" s="7"/>
       <c r="U1566" s="7"/>
       <c r="V1566" s="33" t="s">
-        <v>1425</v>
+        <v>1423</v>
       </c>
     </row>
     <row r="1567" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -61735,7 +61735,7 @@
       <c r="T1567" s="7"/>
       <c r="U1567" s="7"/>
       <c r="V1567" s="33" t="s">
-        <v>1426</v>
+        <v>1424</v>
       </c>
     </row>
     <row r="1568" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -61804,7 +61804,7 @@
       <c r="T1569" s="7"/>
       <c r="U1569" s="7"/>
       <c r="V1569" s="33" t="s">
-        <v>1427</v>
+        <v>1425</v>
       </c>
     </row>
     <row r="1570" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -61839,7 +61839,7 @@
       <c r="T1570" s="7"/>
       <c r="U1570" s="7"/>
       <c r="V1570" s="33" t="s">
-        <v>1428</v>
+        <v>1426</v>
       </c>
     </row>
     <row r="1571" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -61874,7 +61874,7 @@
       <c r="T1571" s="7"/>
       <c r="U1571" s="7"/>
       <c r="V1571" s="33" t="s">
-        <v>1429</v>
+        <v>1427</v>
       </c>
     </row>
     <row r="1572" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -61942,7 +61942,7 @@
       <c r="T1573" s="7"/>
       <c r="U1573" s="7"/>
       <c r="V1573" s="33" t="s">
-        <v>1428</v>
+        <v>1426</v>
       </c>
     </row>
     <row r="1574" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -62048,7 +62048,7 @@
       <c r="T1576" s="7"/>
       <c r="U1576" s="7"/>
       <c r="V1576" s="33" t="s">
-        <v>1391</v>
+        <v>1389</v>
       </c>
     </row>
     <row r="1577" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -62226,7 +62226,7 @@
         <v>72</v>
       </c>
       <c r="V1581" s="33" t="s">
-        <v>1430</v>
+        <v>1428</v>
       </c>
     </row>
     <row r="1582" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -62438,7 +62438,7 @@
         <v>72</v>
       </c>
       <c r="V1588" s="33" t="s">
-        <v>1431</v>
+        <v>1429</v>
       </c>
     </row>
     <row r="1589" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -62570,7 +62570,7 @@
         <v>72</v>
       </c>
       <c r="V1593" s="33" t="s">
-        <v>1432</v>
+        <v>1430</v>
       </c>
     </row>
     <row r="1594" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -63015,7 +63015,7 @@
         <v>72</v>
       </c>
       <c r="V1610" s="33" t="s">
-        <v>1433</v>
+        <v>1431</v>
       </c>
     </row>
     <row r="1611" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -63044,7 +63044,7 @@
         <v>72</v>
       </c>
       <c r="V1611" s="33" t="s">
-        <v>1434</v>
+        <v>1432</v>
       </c>
     </row>
     <row r="1612" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -63151,7 +63151,7 @@
         <v>72</v>
       </c>
       <c r="V1615" s="33" t="s">
-        <v>1435</v>
+        <v>1433</v>
       </c>
     </row>
     <row r="1616" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -63206,7 +63206,7 @@
         <v>72</v>
       </c>
       <c r="V1617" s="33" t="s">
-        <v>1436</v>
+        <v>1434</v>
       </c>
     </row>
     <row r="1618" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -63287,7 +63287,7 @@
         <v>72</v>
       </c>
       <c r="V1620" s="33" t="s">
-        <v>1437</v>
+        <v>1435</v>
       </c>
     </row>
     <row r="1621" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -63458,7 +63458,7 @@
         <v>72</v>
       </c>
       <c r="V1626" s="33" t="s">
-        <v>1438</v>
+        <v>1436</v>
       </c>
     </row>
     <row r="1627" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -63803,7 +63803,7 @@
         <v>73</v>
       </c>
       <c r="V1638" s="33" t="s">
-        <v>1439</v>
+        <v>1437</v>
       </c>
     </row>
     <row r="1639" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -64053,7 +64053,7 @@
         <v>73</v>
       </c>
       <c r="V1647" s="33" t="s">
-        <v>1440</v>
+        <v>1438</v>
       </c>
     </row>
     <row r="1648" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -64307,7 +64307,7 @@
         <v>73</v>
       </c>
       <c r="V1655" s="33" t="s">
-        <v>1441</v>
+        <v>1439</v>
       </c>
     </row>
     <row r="1656" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -64339,7 +64339,7 @@
         <v>72</v>
       </c>
       <c r="V1656" s="33" t="s">
-        <v>1442</v>
+        <v>1440</v>
       </c>
     </row>
     <row r="1657" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -64461,7 +64461,7 @@
         <v>72</v>
       </c>
       <c r="V1660" s="33" t="s">
-        <v>1443</v>
+        <v>1441</v>
       </c>
     </row>
     <row r="1661" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -64528,7 +64528,7 @@
         <v>81</v>
       </c>
       <c r="V1662" s="33" t="s">
-        <v>1444</v>
+        <v>1442</v>
       </c>
     </row>
     <row r="1663" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -64560,7 +64560,7 @@
         <v>73</v>
       </c>
       <c r="V1663" s="33" t="s">
-        <v>1445</v>
+        <v>1443</v>
       </c>
     </row>
     <row r="1664" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -64650,7 +64650,7 @@
         <v>72</v>
       </c>
       <c r="V1666" s="33" t="s">
-        <v>1446</v>
+        <v>1444</v>
       </c>
     </row>
     <row r="1667" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -64685,7 +64685,7 @@
         <v>72</v>
       </c>
       <c r="V1667" s="33" t="s">
-        <v>1447</v>
+        <v>1445</v>
       </c>
     </row>
     <row r="1668" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -64853,7 +64853,7 @@
       </c>
       <c r="U1672" s="7"/>
       <c r="V1672" s="33" t="s">
-        <v>1448</v>
+        <v>1446</v>
       </c>
     </row>
     <row r="1673" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -64976,7 +64976,7 @@
         <v>72</v>
       </c>
       <c r="V1676" s="33" t="s">
-        <v>1449</v>
+        <v>1447</v>
       </c>
     </row>
     <row r="1677" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -65008,7 +65008,7 @@
         <v>72</v>
       </c>
       <c r="V1677" s="33" t="s">
-        <v>1450</v>
+        <v>1448</v>
       </c>
     </row>
     <row r="1678" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -65098,7 +65098,7 @@
         <v>73</v>
       </c>
       <c r="V1680" s="33" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
     </row>
     <row r="1681" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -65133,7 +65133,7 @@
         <v>74</v>
       </c>
       <c r="V1681" s="33" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
     </row>
     <row r="1682" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -65300,7 +65300,7 @@
         <v>73</v>
       </c>
       <c r="V1686" s="33" t="s">
-        <v>1453</v>
+        <v>1451</v>
       </c>
     </row>
     <row r="1687" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -65469,7 +65469,7 @@
         <v>73</v>
       </c>
       <c r="V1691" s="33" t="s">
-        <v>1454</v>
+        <v>1452</v>
       </c>
     </row>
     <row r="1692" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -65501,7 +65501,7 @@
         <v>72</v>
       </c>
       <c r="V1692" s="33" t="s">
-        <v>1455</v>
+        <v>1453</v>
       </c>
     </row>
     <row r="1693" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -65620,7 +65620,7 @@
         <v>72</v>
       </c>
       <c r="V1696" s="33" t="s">
-        <v>1456</v>
+        <v>1454</v>
       </c>
     </row>
     <row r="1697" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -65652,7 +65652,7 @@
         <v>72</v>
       </c>
       <c r="V1697" s="33" t="s">
-        <v>1457</v>
+        <v>1455</v>
       </c>
     </row>
     <row r="1698" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -65683,7 +65683,7 @@
         <v>73</v>
       </c>
       <c r="V1698" s="34" t="s">
-        <v>1486</v>
+        <v>1484</v>
       </c>
     </row>
     <row r="1699" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -65782,7 +65782,7 @@
         <v>72</v>
       </c>
       <c r="V1701" s="33" t="s">
-        <v>1458</v>
+        <v>1456</v>
       </c>
     </row>
     <row r="1702" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -65904,7 +65904,7 @@
         <v>72</v>
       </c>
       <c r="V1705" s="33" t="s">
-        <v>1459</v>
+        <v>1457</v>
       </c>
     </row>
     <row r="1706" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -65967,7 +65967,7 @@
       </c>
       <c r="U1707" s="7"/>
       <c r="V1707" s="33" t="s">
-        <v>1460</v>
+        <v>1458</v>
       </c>
     </row>
     <row r="1708" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -66088,7 +66088,7 @@
         <v>72</v>
       </c>
       <c r="V1711" s="33" t="s">
-        <v>1442</v>
+        <v>1440</v>
       </c>
     </row>
     <row r="1712" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -66152,7 +66152,7 @@
         <v>73</v>
       </c>
       <c r="V1713" s="33" t="s">
-        <v>1461</v>
+        <v>1459</v>
       </c>
     </row>
     <row r="1714" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -66184,7 +66184,7 @@
         <v>72</v>
       </c>
       <c r="V1714" s="33" t="s">
-        <v>1462</v>
+        <v>1460</v>
       </c>
     </row>
     <row r="1715" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -66222,7 +66222,7 @@
         <v>85</v>
       </c>
       <c r="V1715" s="33" t="s">
-        <v>1463</v>
+        <v>1461</v>
       </c>
     </row>
     <row r="1716" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -66435,7 +66435,7 @@
         <v>73</v>
       </c>
       <c r="V1721" s="33" t="s">
-        <v>1439</v>
+        <v>1437</v>
       </c>
     </row>
     <row r="1722" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -66715,7 +66715,7 @@
         <v>73</v>
       </c>
       <c r="V1730" s="33" t="s">
-        <v>1440</v>
+        <v>1438</v>
       </c>
     </row>
     <row r="1731" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -66776,7 +66776,7 @@
         <v>72</v>
       </c>
       <c r="V1732" s="33" t="s">
-        <v>1464</v>
+        <v>1462</v>
       </c>
     </row>
     <row r="1733" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -66914,7 +66914,7 @@
         <v>73</v>
       </c>
       <c r="V1736" s="33" t="s">
-        <v>1465</v>
+        <v>1463</v>
       </c>
     </row>
     <row r="1737" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -67004,7 +67004,7 @@
         <v>72</v>
       </c>
       <c r="V1739" s="33" t="s">
-        <v>1466</v>
+        <v>1464</v>
       </c>
     </row>
     <row r="1740" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -67039,7 +67039,7 @@
         <v>73</v>
       </c>
       <c r="V1740" s="33" t="s">
-        <v>1467</v>
+        <v>1465</v>
       </c>
     </row>
     <row r="1741" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -67132,7 +67132,7 @@
         <v>72</v>
       </c>
       <c r="V1743" s="33" t="s">
-        <v>1468</v>
+        <v>1466</v>
       </c>
     </row>
     <row r="1744" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -67317,7 +67317,7 @@
         <v>73</v>
       </c>
       <c r="V1749" s="33" t="s">
-        <v>1469</v>
+        <v>1467</v>
       </c>
     </row>
     <row r="1750" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -67407,7 +67407,7 @@
         <v>72</v>
       </c>
       <c r="V1752" s="33" t="s">
-        <v>1470</v>
+        <v>1468</v>
       </c>
     </row>
     <row r="1753" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -67564,7 +67564,7 @@
         <v>73</v>
       </c>
       <c r="V1757" s="33" t="s">
-        <v>1471</v>
+        <v>1469</v>
       </c>
     </row>
     <row r="1758" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -67663,7 +67663,7 @@
         <v>72</v>
       </c>
       <c r="V1760" s="33" t="s">
-        <v>1472</v>
+        <v>1470</v>
       </c>
     </row>
     <row r="1761" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -67756,7 +67756,7 @@
         <v>73</v>
       </c>
       <c r="V1763" s="34" t="s">
-        <v>1473</v>
+        <v>1471</v>
       </c>
     </row>
     <row r="1764" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -67878,7 +67878,7 @@
         <v>73</v>
       </c>
       <c r="V1767" s="33" t="s">
-        <v>1474</v>
+        <v>1472</v>
       </c>
     </row>
     <row r="1768" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -68207,7 +68207,7 @@
         <v>73</v>
       </c>
       <c r="V1777" s="33" t="s">
-        <v>1475</v>
+        <v>1473</v>
       </c>
     </row>
     <row r="1778" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -68445,7 +68445,7 @@
         <v>73</v>
       </c>
       <c r="V1785" s="33" t="s">
-        <v>1476</v>
+        <v>1474</v>
       </c>
     </row>
     <row r="1786" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -68626,7 +68626,7 @@
         <v>72</v>
       </c>
       <c r="V1791" s="34" t="s">
-        <v>1477</v>
+        <v>1475</v>
       </c>
     </row>
     <row r="1792" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -68658,7 +68658,7 @@
         <v>73</v>
       </c>
       <c r="V1792" s="33" t="s">
-        <v>1478</v>
+        <v>1476</v>
       </c>
     </row>
     <row r="1793" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -68690,7 +68690,7 @@
         <v>72</v>
       </c>
       <c r="V1793" s="33" t="s">
-        <v>1479</v>
+        <v>1477</v>
       </c>
     </row>
     <row r="1794" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -68725,7 +68725,7 @@
         <v>73</v>
       </c>
       <c r="V1794" s="33" t="s">
-        <v>1480</v>
+        <v>1478</v>
       </c>
     </row>
     <row r="1795" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -68966,7 +68966,7 @@
         <v>73</v>
       </c>
       <c r="V1802" s="33" t="s">
-        <v>1481</v>
+        <v>1479</v>
       </c>
     </row>
     <row r="1803" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -69059,7 +69059,7 @@
         <v>73</v>
       </c>
       <c r="V1805" s="33" t="s">
-        <v>1482</v>
+        <v>1480</v>
       </c>
     </row>
     <row r="1806" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -69263,7 +69263,7 @@
         <v>73</v>
       </c>
       <c r="V1811" s="33" t="s">
-        <v>1483</v>
+        <v>1481</v>
       </c>
     </row>
     <row r="1812" spans="3:22" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
nmv 13 02 2026
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Padam Input Templates/TS 1.4 Padam Input Template.xlsx
+++ b/TS Jatai Working/Padam Input Templates/TS 1.4 Padam Input Template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALL IMP DATA\GitHub\texts\TS Jatai Working\Padam Input Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{217466FC-8EDC-4B59-85A3-239D86CAF043}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDB86AF6-27BC-4948-97D1-5B2616A64642}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6754" uniqueCount="1497">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6750" uniqueCount="1497">
   <si>
     <t>Passage</t>
   </si>
@@ -4450,9 +4450,6 @@
   </si>
   <si>
     <t>praqBiqndanniti# pra - Biqndann</t>
-  </si>
-  <si>
-    <t>vAja#sAtaqvitiq vAja# - sAqtauq</t>
   </si>
   <si>
     <t>gRuqhapa#tiqriti# gRuqha - paqtiqH</t>
@@ -4658,6 +4655,9 @@
   </si>
   <si>
     <t>aqveqpaqyaq itya#vepayaH</t>
+  </si>
+  <si>
+    <t>vAja#sAtAqvitiq vAja# - sAqtauq</t>
   </si>
 </sst>
 </file>
@@ -5342,10 +5342,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V1812"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="O1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A1775" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="N926" sqref="N926"/>
+      <selection pane="bottomLeft" activeCell="V1785" sqref="V1785"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -31322,7 +31322,7 @@
       <c r="T697" s="7"/>
       <c r="U697" s="7"/>
       <c r="V697" s="34" t="s">
-        <v>1494</v>
+        <v>1493</v>
       </c>
     </row>
     <row r="698" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -33413,7 +33413,7 @@
         <v>52</v>
       </c>
       <c r="N758" s="34" t="s">
-        <v>1486</v>
+        <v>1485</v>
       </c>
       <c r="O758" s="6" t="s">
         <v>72</v>
@@ -33632,7 +33632,7 @@
       <c r="T764" s="7"/>
       <c r="U764" s="7"/>
       <c r="V764" s="34" t="s">
-        <v>1495</v>
+        <v>1494</v>
       </c>
     </row>
     <row r="765" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -35105,7 +35105,7 @@
       <c r="T807" s="7"/>
       <c r="U807" s="7"/>
       <c r="V807" s="34" t="s">
-        <v>1487</v>
+        <v>1486</v>
       </c>
     </row>
     <row r="808" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -35908,7 +35908,7 @@
       <c r="T830" s="7"/>
       <c r="U830" s="7"/>
       <c r="V830" s="34" t="s">
-        <v>1482</v>
+        <v>1481</v>
       </c>
     </row>
     <row r="831" spans="6:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -36380,7 +36380,7 @@
       <c r="T844" s="7"/>
       <c r="U844" s="7"/>
       <c r="V844" s="34" t="s">
-        <v>1487</v>
+        <v>1486</v>
       </c>
     </row>
     <row r="845" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -37086,7 +37086,7 @@
         <v>9</v>
       </c>
       <c r="N865" s="34" t="s">
-        <v>1488</v>
+        <v>1487</v>
       </c>
       <c r="O865" s="6" t="s">
         <v>72</v>
@@ -39173,7 +39173,7 @@
         <v>81</v>
       </c>
       <c r="V926" s="34" t="s">
-        <v>1496</v>
+        <v>1495</v>
       </c>
     </row>
     <row r="927" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -39676,7 +39676,7 @@
       <c r="T941" s="7"/>
       <c r="U941" s="7"/>
       <c r="V941" s="34" t="s">
-        <v>1489</v>
+        <v>1488</v>
       </c>
     </row>
     <row r="942" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -40690,7 +40690,7 @@
         <v>80</v>
       </c>
       <c r="T971" s="61" t="s">
-        <v>1485</v>
+        <v>1484</v>
       </c>
       <c r="U971" s="7"/>
       <c r="V971" s="33" t="s">
@@ -53535,7 +53535,7 @@
         <v>1</v>
       </c>
       <c r="N1344" s="34" t="s">
-        <v>1490</v>
+        <v>1489</v>
       </c>
       <c r="O1344" s="6"/>
       <c r="P1344" s="7"/>
@@ -59079,7 +59079,7 @@
       <c r="T1491" s="7"/>
       <c r="U1491" s="7"/>
       <c r="V1491" s="34" t="s">
-        <v>1483</v>
+        <v>1482</v>
       </c>
     </row>
     <row r="1492" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -59337,7 +59337,7 @@
         <v>8</v>
       </c>
       <c r="N1499" s="34" t="s">
-        <v>1491</v>
+        <v>1490</v>
       </c>
       <c r="O1499" s="6" t="s">
         <v>72</v>
@@ -59689,7 +59689,7 @@
       <c r="T1508" s="7"/>
       <c r="U1508" s="7"/>
       <c r="V1508" s="34" t="s">
-        <v>1492</v>
+        <v>1491</v>
       </c>
     </row>
     <row r="1509" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -60639,7 +60639,7 @@
       <c r="T1536" s="7"/>
       <c r="U1536" s="7"/>
       <c r="V1536" s="34" t="s">
-        <v>1493</v>
+        <v>1492</v>
       </c>
     </row>
     <row r="1537" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -65683,7 +65683,7 @@
         <v>73</v>
       </c>
       <c r="V1698" s="34" t="s">
-        <v>1484</v>
+        <v>1483</v>
       </c>
     </row>
     <row r="1699" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -68444,8 +68444,8 @@
       <c r="P1785" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="V1785" s="33" t="s">
-        <v>1474</v>
+      <c r="V1785" s="34" t="s">
+        <v>1496</v>
       </c>
     </row>
     <row r="1786" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -68626,7 +68626,7 @@
         <v>72</v>
       </c>
       <c r="V1791" s="34" t="s">
-        <v>1475</v>
+        <v>1474</v>
       </c>
     </row>
     <row r="1792" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -68658,7 +68658,7 @@
         <v>73</v>
       </c>
       <c r="V1792" s="33" t="s">
-        <v>1476</v>
+        <v>1475</v>
       </c>
     </row>
     <row r="1793" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -68690,7 +68690,7 @@
         <v>72</v>
       </c>
       <c r="V1793" s="33" t="s">
-        <v>1477</v>
+        <v>1476</v>
       </c>
     </row>
     <row r="1794" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -68725,7 +68725,7 @@
         <v>73</v>
       </c>
       <c r="V1794" s="33" t="s">
-        <v>1478</v>
+        <v>1477</v>
       </c>
     </row>
     <row r="1795" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -68966,7 +68966,7 @@
         <v>73</v>
       </c>
       <c r="V1802" s="33" t="s">
-        <v>1479</v>
+        <v>1478</v>
       </c>
     </row>
     <row r="1803" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -69059,7 +69059,7 @@
         <v>73</v>
       </c>
       <c r="V1805" s="33" t="s">
-        <v>1480</v>
+        <v>1479</v>
       </c>
     </row>
     <row r="1806" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -69263,7 +69263,7 @@
         <v>73</v>
       </c>
       <c r="V1811" s="33" t="s">
-        <v>1481</v>
+        <v>1480</v>
       </c>
     </row>
     <row r="1812" spans="3:22" x14ac:dyDescent="0.25">

</xml_diff>